<commit_message>
GAP SHEET - Added Description for Changes
</commit_message>
<xml_diff>
--- a/Nphies-GapSheetV2.8.xlsx
+++ b/Nphies-GapSheetV2.8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alqarnimo\Documents\midtables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khanpa\git\midtables-script\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="2231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="2235">
   <si>
     <t>FieldName</t>
   </si>
@@ -7037,9 +7037,6 @@
     <t>Encounter -&gt; Priority - LOV Updated.</t>
   </si>
   <si>
-    <t>It can be a Scientific Code or GTIN Code For the drug.</t>
-  </si>
-  <si>
     <t>patient-request</t>
   </si>
   <si>
@@ -7050,9 +7047,6 @@
   </si>
   <si>
     <t>Generic</t>
-  </si>
-  <si>
-    <t>prescibedDrugCode</t>
   </si>
   <si>
     <t>NPHIES_CLAIMITEM -&gt; prescibedDrugCode</t>
@@ -7108,59 +7102,6 @@
     <t>The name of the referring provider.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This is the Prescription reference Number is optional in the claim type is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"pharmacy"</t>
-    </r>
-  </si>
-  <si>
-    <t>prescription</t>
-  </si>
-  <si>
-    <t>pharmacistSelectionReason</t>
-  </si>
-  <si>
-    <t>pharmacistSubstitute</t>
-  </si>
-  <si>
-    <t>reasonPharmacistSubstitute</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is mandatory if the claim type is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"pharmacy"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ,This is the pharmacist selection reason when you can choose the type of drug</t>
-    </r>
-  </si>
-  <si>
     <t>PharmacistSelectionReason</t>
   </si>
   <si>
@@ -7233,9 +7174,6 @@
     <t>Added NPHIES_CLAIMITEM -&gt; REASONPHARMACISTSUBSTITUTE</t>
   </si>
   <si>
-    <t>ADDED NPHIES_CLAIMITEM -&gt; PHARMACISTSELECTIONREASON</t>
-  </si>
-  <si>
     <t>Added NPHIES_CLAIMITEMDETAILS -&gt; PHARMACISTSELECTIONREASON</t>
   </si>
   <si>
@@ -7246,6 +7184,45 @@
   </si>
   <si>
     <t>ADDED NPHIES_CLAIMITEMDETAILS -&gt; PRESCIBEDDRUGCODE</t>
+  </si>
+  <si>
+    <t>PrescibedDrugCode</t>
+  </si>
+  <si>
+    <t>PharmacistSubstitute</t>
+  </si>
+  <si>
+    <t>ReasonPharmacistSubstitute</t>
+  </si>
+  <si>
+    <t>PrescribedDrugCode</t>
+  </si>
+  <si>
+    <t>Reasons from the list - for substitute by the pharmacist</t>
+  </si>
+  <si>
+    <t>Reason, if it is not from the pharmacist substitute list - for substitute by the pharmacist</t>
+  </si>
+  <si>
+    <t>Prescribed Medication, as per the Physician. It can be a Scientific Code or GTIN Code.</t>
+  </si>
+  <si>
+    <t>ServiceCode</t>
+  </si>
+  <si>
+    <t>ServiceDesc</t>
+  </si>
+  <si>
+    <t>This is mandatory if the claim type is "pharmacy" ,This is the pharmacist selection reason while choosing the type of drug</t>
+  </si>
+  <si>
+    <t>PRESCRIPTION</t>
+  </si>
+  <si>
+    <t>This is the Prescription reference Number is optional in the claim type is "pharmacy"</t>
+  </si>
+  <si>
+    <t>Added NPHIES_CLAIMITEM -&gt; PRESCIBEDDRUGCODE</t>
   </si>
 </sst>
 </file>
@@ -7428,7 +7405,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7510,6 +7487,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5C7F75"/>
         <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -7817,7 +7799,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -7838,8 +7820,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -8162,17 +8145,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="17"/>
+    <xf numFmtId="49" fontId="2" fillId="15" borderId="1" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="17" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8183,14 +8173,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8201,20 +8203,11 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8231,18 +8224,9 @@
     <xf numFmtId="0" fontId="20" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
+    <cellStyle name="Accent6" xfId="17" builtinId="49"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="12"/>
     <cellStyle name="Hyperlink 3" xfId="3"/>
@@ -8604,7 +8588,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8643,7 +8627,7 @@
       <c r="B3" t="s">
         <v>1936</v>
       </c>
-      <c r="C3" s="144">
+      <c r="C3" s="145">
         <v>44636</v>
       </c>
     </row>
@@ -8652,10 +8636,10 @@
       <c r="B4" t="s">
         <v>1939</v>
       </c>
-      <c r="C4" s="144"/>
+      <c r="C4" s="145"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="145">
+      <c r="A5" s="146">
         <v>2.4</v>
       </c>
       <c r="B5" t="s">
@@ -8663,7 +8647,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="145"/>
+      <c r="A6" s="146"/>
       <c r="B6" t="s">
         <v>2071</v>
       </c>
@@ -8672,31 +8656,31 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="145"/>
+      <c r="A7" s="146"/>
       <c r="B7" t="s">
         <v>2072</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="145"/>
+      <c r="A8" s="146"/>
       <c r="B8" t="s">
         <v>2073</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="145"/>
+      <c r="A9" s="146"/>
       <c r="B9" t="s">
         <v>2074</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="145"/>
+      <c r="A10" s="146"/>
       <c r="B10" t="s">
         <v>2075</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="145">
+      <c r="A12" s="146">
         <v>2.5</v>
       </c>
       <c r="B12" t="s">
@@ -8707,39 +8691,39 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="145"/>
+      <c r="A13" s="146"/>
       <c r="B13" t="s">
         <v>2142</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="145"/>
+      <c r="A14" s="146"/>
       <c r="B14" t="s">
         <v>2143</v>
       </c>
       <c r="C14" s="125"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="145"/>
+      <c r="A15" s="146"/>
       <c r="B15" t="s">
         <v>2156</v>
       </c>
       <c r="C15" s="125"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="145"/>
+      <c r="A16" s="146"/>
       <c r="B16" t="s">
         <v>2152</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="145"/>
+      <c r="A17" s="146"/>
       <c r="B17" t="s">
         <v>2144</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="145"/>
+      <c r="A18" s="146"/>
       <c r="B18" t="s">
         <v>2145</v>
       </c>
@@ -8784,12 +8768,12 @@
     </row>
     <row r="27" spans="1:3">
       <c r="B27" t="s">
-        <v>2187</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" t="s">
-        <v>2186</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -8797,12 +8781,12 @@
         <v>2.7</v>
       </c>
       <c r="B30" t="s">
-        <v>2190</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" t="s">
-        <v>2191</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -8810,56 +8794,56 @@
         <v>2.8</v>
       </c>
       <c r="B33" t="s">
-        <v>2222</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="B34" s="10" t="s">
-        <v>2223</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="B35" t="s">
-        <v>2224</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" t="s">
-        <v>2225</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="B37" t="s">
-        <v>2226</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="143"/>
+      <c r="A38" s="138"/>
       <c r="B38" s="10" t="s">
-        <v>2227</v>
-      </c>
-      <c r="C38" s="143"/>
+        <v>2218</v>
+      </c>
+      <c r="C38" s="138"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="143"/>
+      <c r="A39" s="138"/>
       <c r="B39" t="s">
-        <v>2228</v>
-      </c>
-      <c r="C39" s="143"/>
+        <v>2219</v>
+      </c>
+      <c r="C39" s="138"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="143"/>
+      <c r="A40" s="138"/>
       <c r="B40" t="s">
-        <v>2229</v>
-      </c>
-      <c r="C40" s="143"/>
+        <v>2220</v>
+      </c>
+      <c r="C40" s="138"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="143"/>
+      <c r="A41" s="138"/>
       <c r="B41" t="s">
-        <v>2230</v>
-      </c>
-      <c r="C41" s="143"/>
+        <v>2221</v>
+      </c>
+      <c r="C41" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9555,7 +9539,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="161" t="s">
         <v>2043</v>
       </c>
       <c r="B2" s="89" t="s">
@@ -9566,49 +9550,49 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="159"/>
+      <c r="A3" s="161"/>
       <c r="B3" t="s">
         <v>1694</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="159"/>
+      <c r="A4" s="161"/>
       <c r="B4" t="s">
         <v>1695</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="159"/>
+      <c r="A5" s="161"/>
       <c r="B5" t="s">
         <v>1696</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="159"/>
+      <c r="A6" s="161"/>
       <c r="B6" t="s">
         <v>1697</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="159"/>
+      <c r="A7" s="161"/>
       <c r="B7" t="s">
         <v>1698</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="159"/>
+      <c r="A8" s="161"/>
       <c r="B8" t="s">
         <v>1701</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="159"/>
+      <c r="A9" s="161"/>
       <c r="B9" t="s">
         <v>1699</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1">
-      <c r="A11" s="159" t="s">
+      <c r="A11" s="161" t="s">
         <v>2044</v>
       </c>
       <c r="B11" s="89" t="s">
@@ -9616,43 +9600,43 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="159"/>
+      <c r="A12" s="161"/>
       <c r="B12" s="89" t="s">
         <v>1694</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="159"/>
+      <c r="A13" s="161"/>
       <c r="B13" t="s">
         <v>1695</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="159"/>
+      <c r="A14" s="161"/>
       <c r="B14" t="s">
         <v>1696</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="159"/>
+      <c r="A15" s="161"/>
       <c r="B15" t="s">
         <v>1697</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="159"/>
+      <c r="A16" s="161"/>
       <c r="B16" s="116" t="s">
         <v>1700</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="159"/>
+      <c r="A17" s="161"/>
       <c r="B17" s="80" t="s">
         <v>1701</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1">
-      <c r="A19" s="160" t="s">
+      <c r="A19" s="162" t="s">
         <v>2045</v>
       </c>
       <c r="B19" s="89" t="s">
@@ -9660,49 +9644,49 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="160"/>
+      <c r="A20" s="162"/>
       <c r="B20" s="89" t="s">
         <v>1694</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="160"/>
+      <c r="A21" s="162"/>
       <c r="B21" s="89" t="s">
         <v>1695</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="160"/>
+      <c r="A22" s="162"/>
       <c r="B22" s="89" t="s">
         <v>1696</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="160"/>
+      <c r="A23" s="162"/>
       <c r="B23" s="89" t="s">
         <v>1697</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="160"/>
+      <c r="A24" s="162"/>
       <c r="B24" s="90" t="s">
         <v>1699</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="160"/>
+      <c r="A25" s="162"/>
       <c r="B25" s="116" t="s">
         <v>1700</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="160"/>
+      <c r="A26" s="162"/>
       <c r="B26" s="80" t="s">
         <v>1701</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="159" t="s">
+      <c r="A28" s="161" t="s">
         <v>2046</v>
       </c>
       <c r="B28" s="80" t="s">
@@ -9710,19 +9694,19 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="159"/>
+      <c r="A29" s="161"/>
       <c r="B29" t="s">
         <v>1700</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="159"/>
+      <c r="A30" s="161"/>
       <c r="B30" s="80" t="s">
         <v>1701</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1">
-      <c r="A32" s="160" t="s">
+      <c r="A32" s="162" t="s">
         <v>2047</v>
       </c>
       <c r="B32" s="89" t="s">
@@ -9730,7 +9714,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="160"/>
+      <c r="A33" s="162"/>
       <c r="B33" s="90" t="s">
         <v>1699</v>
       </c>
@@ -9786,7 +9770,7 @@
       <c r="C2" s="108" t="s">
         <v>1986</v>
       </c>
-      <c r="D2" s="161" t="s">
+      <c r="D2" s="163" t="s">
         <v>1700</v>
       </c>
     </row>
@@ -9800,7 +9784,7 @@
       <c r="C3" s="108" t="s">
         <v>1988</v>
       </c>
-      <c r="D3" s="161"/>
+      <c r="D3" s="163"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="108">
@@ -9812,7 +9796,7 @@
       <c r="C4" s="108" t="s">
         <v>1990</v>
       </c>
-      <c r="D4" s="161"/>
+      <c r="D4" s="163"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="108">
@@ -9824,7 +9808,7 @@
       <c r="C5" s="108" t="s">
         <v>1992</v>
       </c>
-      <c r="D5" s="161"/>
+      <c r="D5" s="163"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="108">
@@ -9836,7 +9820,7 @@
       <c r="C6" s="108" t="s">
         <v>1994</v>
       </c>
-      <c r="D6" s="161"/>
+      <c r="D6" s="163"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="108">
@@ -9862,7 +9846,7 @@
       <c r="C8" s="108" t="s">
         <v>1998</v>
       </c>
-      <c r="D8" s="161" t="s">
+      <c r="D8" s="163" t="s">
         <v>1700</v>
       </c>
     </row>
@@ -9876,7 +9860,7 @@
       <c r="C9" s="108" t="s">
         <v>2000</v>
       </c>
-      <c r="D9" s="161"/>
+      <c r="D9" s="163"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="108">
@@ -9888,7 +9872,7 @@
       <c r="C10" s="108" t="s">
         <v>2002</v>
       </c>
-      <c r="D10" s="161"/>
+      <c r="D10" s="163"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="108">
@@ -9900,7 +9884,7 @@
       <c r="C11" s="108" t="s">
         <v>2004</v>
       </c>
-      <c r="D11" s="161"/>
+      <c r="D11" s="163"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="108">
@@ -9912,7 +9896,7 @@
       <c r="C12" s="108" t="s">
         <v>2006</v>
       </c>
-      <c r="D12" s="161"/>
+      <c r="D12" s="163"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="108">
@@ -9924,7 +9908,7 @@
       <c r="C13" s="108" t="s">
         <v>2008</v>
       </c>
-      <c r="D13" s="161"/>
+      <c r="D13" s="163"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="108">
@@ -9936,7 +9920,7 @@
       <c r="C14" s="108" t="s">
         <v>2010</v>
       </c>
-      <c r="D14" s="161"/>
+      <c r="D14" s="163"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="108">
@@ -9948,7 +9932,7 @@
       <c r="C15" s="108" t="s">
         <v>2012</v>
       </c>
-      <c r="D15" s="161"/>
+      <c r="D15" s="163"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="108">
@@ -9960,7 +9944,7 @@
       <c r="C16" s="108" t="s">
         <v>2014</v>
       </c>
-      <c r="D16" s="161"/>
+      <c r="D16" s="163"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="108">
@@ -9972,7 +9956,7 @@
       <c r="C17" s="108" t="s">
         <v>2016</v>
       </c>
-      <c r="D17" s="161"/>
+      <c r="D17" s="163"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="108">
@@ -9984,7 +9968,7 @@
       <c r="C18" s="108" t="s">
         <v>2018</v>
       </c>
-      <c r="D18" s="161"/>
+      <c r="D18" s="163"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="108">
@@ -9996,7 +9980,7 @@
       <c r="C19" s="108" t="s">
         <v>2020</v>
       </c>
-      <c r="D19" s="161"/>
+      <c r="D19" s="163"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="108">
@@ -10008,7 +9992,7 @@
       <c r="C20" s="108" t="s">
         <v>2022</v>
       </c>
-      <c r="D20" s="161"/>
+      <c r="D20" s="163"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="108">
@@ -10067,10 +10051,10 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="162" t="s">
+      <c r="A25" s="164" t="s">
         <v>2031</v>
       </c>
-      <c r="B25" s="162"/>
+      <c r="B25" s="164"/>
       <c r="C25" s="110" t="s">
         <v>2032</v>
       </c>
@@ -10461,8 +10445,8 @@
   <dimension ref="A1:H199"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B131" sqref="B131"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11074,32 +11058,32 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="139" customFormat="1">
-      <c r="B46" s="140" t="s">
+    <row r="46" spans="1:8">
+      <c r="B46" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" t="s">
         <v>2192</v>
       </c>
-      <c r="C46" s="141" t="s">
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C47" t="s">
         <v>77</v>
       </c>
-      <c r="D46" s="141" t="s">
+      <c r="D47" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="142" t="s">
-        <v>2194</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="139" customFormat="1">
-      <c r="B47" s="140" t="s">
+      <c r="E47" t="s">
         <v>2193</v>
-      </c>
-      <c r="C47" s="141" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="141" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="142" t="s">
-        <v>2195</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -11359,18 +11343,18 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="82" customFormat="1">
-      <c r="B65" s="82" t="s">
-        <v>2197</v>
-      </c>
-      <c r="C65" s="82" t="s">
+    <row r="65" spans="1:8" s="142" customFormat="1">
+      <c r="B65" s="142" t="s">
+        <v>2232</v>
+      </c>
+      <c r="C65" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="133" t="s">
+      <c r="D65" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="E65" s="102" t="s">
-        <v>2196</v>
+      <c r="E65" s="144" t="s">
+        <v>2233</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -11704,7 +11688,7 @@
     </row>
     <row r="90" spans="1:8" ht="28.8">
       <c r="B90" s="21" t="s">
-        <v>14</v>
+        <v>2229</v>
       </c>
       <c r="C90" t="s">
         <v>77</v>
@@ -11720,7 +11704,7 @@
     </row>
     <row r="91" spans="1:8">
       <c r="B91" s="20" t="s">
-        <v>15</v>
+        <v>2230</v>
       </c>
       <c r="C91" t="s">
         <v>77</v>
@@ -11762,20 +11746,20 @@
       <c r="F93" s="64"/>
       <c r="H93" s="13"/>
     </row>
-    <row r="94" spans="1:8">
-      <c r="B94" t="s">
-        <v>2185</v>
-      </c>
-      <c r="C94" t="s">
+    <row r="94" spans="1:8" s="142" customFormat="1">
+      <c r="B94" s="142" t="s">
+        <v>2222</v>
+      </c>
+      <c r="C94" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="E94" t="s">
-        <v>2180</v>
-      </c>
-      <c r="H94" s="13"/>
+      <c r="E94" s="142" t="s">
+        <v>2228</v>
+      </c>
+      <c r="H94" s="143"/>
     </row>
     <row r="95" spans="1:8">
       <c r="B95" t="s">
@@ -11989,42 +11973,48 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="110" spans="2:8">
-      <c r="B110" t="s">
-        <v>2198</v>
-      </c>
-      <c r="C110" t="s">
+    <row r="110" spans="2:8" s="142" customFormat="1">
+      <c r="B110" s="142" t="s">
+        <v>2194</v>
+      </c>
+      <c r="C110" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="E110" t="s">
-        <v>2201</v>
-      </c>
-    </row>
-    <row r="111" spans="2:8">
-      <c r="B111" t="s">
-        <v>2199</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="E110" s="142" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" s="142" customFormat="1">
+      <c r="B111" s="142" t="s">
+        <v>2223</v>
+      </c>
+      <c r="C111" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="142" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="112" spans="2:8">
-      <c r="B112" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C112" t="s">
+      <c r="E111" s="142" t="s">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" s="142" customFormat="1">
+      <c r="B112" s="142" t="s">
+        <v>2224</v>
+      </c>
+      <c r="C112" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H112" s="10"/>
+      <c r="E112" s="142" t="s">
+        <v>2227</v>
+      </c>
+      <c r="H112" s="144"/>
     </row>
     <row r="113" spans="1:8" ht="28.8">
       <c r="A113" s="6" t="s">
@@ -12094,7 +12084,7 @@
     </row>
     <row r="118" spans="1:8">
       <c r="B118" s="21" t="s">
-        <v>14</v>
+        <v>2229</v>
       </c>
       <c r="C118" t="s">
         <v>77</v>
@@ -12110,7 +12100,7 @@
     </row>
     <row r="119" spans="1:8">
       <c r="B119" s="20" t="s">
-        <v>15</v>
+        <v>2230</v>
       </c>
       <c r="C119" t="s">
         <v>77</v>
@@ -12232,56 +12222,62 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
-      <c r="B128" t="s">
-        <v>2198</v>
-      </c>
-      <c r="C128" t="s">
+    <row r="128" spans="1:8" s="142" customFormat="1">
+      <c r="B128" s="142" t="s">
+        <v>2194</v>
+      </c>
+      <c r="C128" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="E128" t="s">
-        <v>2201</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8">
-      <c r="B129" t="s">
-        <v>2199</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="E128" s="142" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" s="142" customFormat="1">
+      <c r="B129" s="142" t="s">
+        <v>2223</v>
+      </c>
+      <c r="C129" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="142" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
-      <c r="B130" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="E129" s="142" t="s">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" s="142" customFormat="1">
+      <c r="B130" s="142" t="s">
+        <v>2224</v>
+      </c>
+      <c r="C130" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="142" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="131" spans="1:8">
-      <c r="B131" t="s">
-        <v>2185</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="E130" s="142" t="s">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" s="142" customFormat="1">
+      <c r="B131" s="142" t="s">
+        <v>2225</v>
+      </c>
+      <c r="C131" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="E131" t="s">
-        <v>2180</v>
-      </c>
-      <c r="H131" s="13"/>
+      <c r="E131" s="142" t="s">
+        <v>2228</v>
+      </c>
+      <c r="H131" s="143"/>
     </row>
     <row r="132" spans="1:8">
       <c r="A132" s="19" t="s">
@@ -12705,7 +12701,7 @@
         <v>72</v>
       </c>
       <c r="E165" t="s">
-        <v>2188</v>
+        <v>2186</v>
       </c>
       <c r="F165" t="s">
         <v>120</v>
@@ -13215,8 +13211,8 @@
   <dimension ref="A1:F189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A185" sqref="A185"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13247,10 +13243,10 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="146">
+      <c r="A2" s="147">
         <v>1</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="155" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -13264,8 +13260,8 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="146"/>
-      <c r="B3" s="147"/>
+      <c r="A3" s="147"/>
+      <c r="B3" s="153"/>
       <c r="C3" s="26" t="s">
         <v>842</v>
       </c>
@@ -13277,8 +13273,8 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="146"/>
-      <c r="B4" s="147"/>
+      <c r="A4" s="147"/>
+      <c r="B4" s="153"/>
       <c r="C4" s="26" t="s">
         <v>845</v>
       </c>
@@ -13290,8 +13286,8 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="146"/>
-      <c r="B5" s="147"/>
+      <c r="A5" s="147"/>
+      <c r="B5" s="153"/>
       <c r="C5" s="26" t="s">
         <v>847</v>
       </c>
@@ -13303,8 +13299,8 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="146"/>
-      <c r="B6" s="147"/>
+      <c r="A6" s="147"/>
+      <c r="B6" s="153"/>
       <c r="C6" s="26" t="s">
         <v>850</v>
       </c>
@@ -13316,8 +13312,8 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="146"/>
-      <c r="B7" s="147"/>
+      <c r="A7" s="147"/>
+      <c r="B7" s="153"/>
       <c r="C7" s="26" t="s">
         <v>852</v>
       </c>
@@ -13329,8 +13325,8 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="146"/>
-      <c r="B8" s="147"/>
+      <c r="A8" s="147"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="26" t="s">
         <v>854</v>
       </c>
@@ -13342,8 +13338,8 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="146"/>
-      <c r="B9" s="147"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="26" t="s">
         <v>856</v>
       </c>
@@ -13355,10 +13351,10 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="149" t="s">
+      <c r="A10" s="152" t="s">
         <v>858</v>
       </c>
-      <c r="B10" s="147" t="s">
+      <c r="B10" s="153" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="26" t="s">
@@ -13372,8 +13368,8 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="149"/>
-      <c r="B11" s="147"/>
+      <c r="A11" s="152"/>
+      <c r="B11" s="153"/>
       <c r="C11" s="26" t="s">
         <v>861</v>
       </c>
@@ -13385,8 +13381,8 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="149"/>
-      <c r="B12" s="147"/>
+      <c r="A12" s="152"/>
+      <c r="B12" s="153"/>
       <c r="C12" s="26" t="s">
         <v>864</v>
       </c>
@@ -13398,8 +13394,8 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="149"/>
-      <c r="B13" s="147"/>
+      <c r="A13" s="152"/>
+      <c r="B13" s="153"/>
       <c r="C13" s="26" t="s">
         <v>847</v>
       </c>
@@ -13411,8 +13407,8 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="149"/>
-      <c r="B14" s="147"/>
+      <c r="A14" s="152"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="26" t="s">
         <v>869</v>
       </c>
@@ -13424,10 +13420,10 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="149" t="s">
+      <c r="A15" s="152" t="s">
         <v>872</v>
       </c>
-      <c r="B15" s="151" t="s">
+      <c r="B15" s="156" t="s">
         <v>873</v>
       </c>
       <c r="C15" s="26" t="s">
@@ -13441,8 +13437,8 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="149"/>
-      <c r="B16" s="152"/>
+      <c r="A16" s="152"/>
+      <c r="B16" s="157"/>
       <c r="C16" s="26" t="s">
         <v>877</v>
       </c>
@@ -13454,8 +13450,8 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="149"/>
-      <c r="B17" s="152"/>
+      <c r="A17" s="152"/>
+      <c r="B17" s="157"/>
       <c r="C17" s="26" t="s">
         <v>880</v>
       </c>
@@ -13467,8 +13463,8 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="149"/>
-      <c r="B18" s="152"/>
+      <c r="A18" s="152"/>
+      <c r="B18" s="157"/>
       <c r="C18" s="26" t="s">
         <v>883</v>
       </c>
@@ -13480,8 +13476,8 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="149"/>
-      <c r="B19" s="152"/>
+      <c r="A19" s="152"/>
+      <c r="B19" s="157"/>
       <c r="C19" s="26" t="s">
         <v>886</v>
       </c>
@@ -13493,8 +13489,8 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="149"/>
-      <c r="B20" s="152"/>
+      <c r="A20" s="152"/>
+      <c r="B20" s="157"/>
       <c r="C20" s="26" t="s">
         <v>889</v>
       </c>
@@ -13506,8 +13502,8 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="149"/>
-      <c r="B21" s="150"/>
+      <c r="A21" s="152"/>
+      <c r="B21" s="155"/>
       <c r="C21" s="26" t="s">
         <v>892</v>
       </c>
@@ -13519,10 +13515,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.8">
-      <c r="A22" s="148">
+      <c r="A22" s="158">
         <v>4</v>
       </c>
-      <c r="B22" s="147" t="s">
+      <c r="B22" s="153" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="27" t="s">
@@ -13536,8 +13532,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.2">
-      <c r="A23" s="146"/>
-      <c r="B23" s="147"/>
+      <c r="A23" s="147"/>
+      <c r="B23" s="153"/>
       <c r="C23" s="26" t="s">
         <v>898</v>
       </c>
@@ -13549,10 +13545,10 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="146">
+      <c r="A24" s="147">
         <v>5</v>
       </c>
-      <c r="B24" s="147" t="s">
+      <c r="B24" s="153" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="28" t="s">
@@ -13566,8 +13562,8 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="146"/>
-      <c r="B25" s="147"/>
+      <c r="A25" s="147"/>
+      <c r="B25" s="153"/>
       <c r="C25" s="26" t="s">
         <v>903</v>
       </c>
@@ -13579,8 +13575,8 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="146"/>
-      <c r="B26" s="147"/>
+      <c r="A26" s="147"/>
+      <c r="B26" s="153"/>
       <c r="C26" s="26" t="s">
         <v>906</v>
       </c>
@@ -13592,8 +13588,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8">
-      <c r="A27" s="146"/>
-      <c r="B27" s="147"/>
+      <c r="A27" s="147"/>
+      <c r="B27" s="153"/>
       <c r="C27" s="28" t="s">
         <v>909</v>
       </c>
@@ -13605,8 +13601,8 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="146"/>
-      <c r="B28" s="147"/>
+      <c r="A28" s="147"/>
+      <c r="B28" s="153"/>
       <c r="C28" s="26" t="s">
         <v>911</v>
       </c>
@@ -13618,10 +13614,10 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="149" t="s">
+      <c r="A29" s="152" t="s">
         <v>914</v>
       </c>
-      <c r="B29" s="147" t="s">
+      <c r="B29" s="153" t="s">
         <v>915</v>
       </c>
       <c r="C29" s="26" t="s">
@@ -13635,8 +13631,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8">
-      <c r="A30" s="149"/>
-      <c r="B30" s="147"/>
+      <c r="A30" s="152"/>
+      <c r="B30" s="153"/>
       <c r="C30" s="26" t="s">
         <v>918</v>
       </c>
@@ -13648,8 +13644,8 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="149"/>
-      <c r="B31" s="147"/>
+      <c r="A31" s="152"/>
+      <c r="B31" s="153"/>
       <c r="C31" s="26" t="s">
         <v>920</v>
       </c>
@@ -13661,10 +13657,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="43.8" thickBot="1">
-      <c r="A32" s="146">
+      <c r="A32" s="147">
         <v>7</v>
       </c>
-      <c r="B32" s="147" t="s">
+      <c r="B32" s="153" t="s">
         <v>86</v>
       </c>
       <c r="C32" s="28" t="s">
@@ -13678,8 +13674,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="58.2" thickBot="1">
-      <c r="A33" s="146"/>
-      <c r="B33" s="147"/>
+      <c r="A33" s="147"/>
+      <c r="B33" s="153"/>
       <c r="C33" s="26" t="s">
         <v>926</v>
       </c>
@@ -13691,8 +13687,8 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="146"/>
-      <c r="B34" s="147"/>
+      <c r="A34" s="147"/>
+      <c r="B34" s="153"/>
       <c r="C34" s="26" t="s">
         <v>929</v>
       </c>
@@ -13704,8 +13700,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.2">
-      <c r="A35" s="146"/>
-      <c r="B35" s="147"/>
+      <c r="A35" s="147"/>
+      <c r="B35" s="153"/>
       <c r="C35" s="28" t="s">
         <v>932</v>
       </c>
@@ -13717,8 +13713,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8">
-      <c r="A36" s="146"/>
-      <c r="B36" s="147"/>
+      <c r="A36" s="147"/>
+      <c r="B36" s="153"/>
       <c r="C36" s="26" t="s">
         <v>935</v>
       </c>
@@ -13730,10 +13726,10 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="149" t="s">
+      <c r="A37" s="152" t="s">
         <v>938</v>
       </c>
-      <c r="B37" s="147" t="s">
+      <c r="B37" s="153" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="32">
@@ -13747,8 +13743,8 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="149"/>
-      <c r="B38" s="147"/>
+      <c r="A38" s="152"/>
+      <c r="B38" s="153"/>
       <c r="C38" s="32">
         <v>576</v>
       </c>
@@ -13760,8 +13756,8 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="149"/>
-      <c r="B39" s="147"/>
+      <c r="A39" s="152"/>
+      <c r="B39" s="153"/>
       <c r="C39" s="32">
         <v>356</v>
       </c>
@@ -13773,8 +13769,8 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="149"/>
-      <c r="B40" s="147"/>
+      <c r="A40" s="152"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="32">
         <v>621</v>
       </c>
@@ -13786,8 +13782,8 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="149"/>
-      <c r="B41" s="147"/>
+      <c r="A41" s="152"/>
+      <c r="B41" s="153"/>
       <c r="C41" s="32">
         <v>179</v>
       </c>
@@ -13799,10 +13795,10 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="149" t="s">
+      <c r="A42" s="152" t="s">
         <v>945</v>
       </c>
-      <c r="B42" s="147" t="s">
+      <c r="B42" s="153" t="s">
         <v>87</v>
       </c>
       <c r="C42" s="27"/>
@@ -13810,8 +13806,8 @@
       <c r="E42" s="32"/>
     </row>
     <row r="43" spans="1:5" s="126" customFormat="1">
-      <c r="A43" s="149"/>
-      <c r="B43" s="147"/>
+      <c r="A43" s="152"/>
+      <c r="B43" s="153"/>
       <c r="C43" s="135" t="s">
         <v>946</v>
       </c>
@@ -13823,8 +13819,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="126" customFormat="1">
-      <c r="A44" s="149"/>
-      <c r="B44" s="147"/>
+      <c r="A44" s="152"/>
+      <c r="B44" s="153"/>
       <c r="C44" s="135" t="s">
         <v>949</v>
       </c>
@@ -13836,10 +13832,10 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="149" t="s">
+      <c r="A45" s="152" t="s">
         <v>952</v>
       </c>
-      <c r="B45" s="147" t="s">
+      <c r="B45" s="153" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="27" t="s">
@@ -13853,8 +13849,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="28.8">
-      <c r="A46" s="149"/>
-      <c r="B46" s="147"/>
+      <c r="A46" s="152"/>
+      <c r="B46" s="153"/>
       <c r="C46" s="26" t="s">
         <v>956</v>
       </c>
@@ -13866,8 +13862,8 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="149"/>
-      <c r="B47" s="147"/>
+      <c r="A47" s="152"/>
+      <c r="B47" s="153"/>
       <c r="C47" s="26" t="s">
         <v>959</v>
       </c>
@@ -13879,8 +13875,8 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="149"/>
-      <c r="B48" s="147"/>
+      <c r="A48" s="152"/>
+      <c r="B48" s="153"/>
       <c r="C48" s="26" t="s">
         <v>962</v>
       </c>
@@ -13892,8 +13888,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="28.8">
-      <c r="A49" s="149"/>
-      <c r="B49" s="147"/>
+      <c r="A49" s="152"/>
+      <c r="B49" s="153"/>
       <c r="C49" s="26" t="s">
         <v>965</v>
       </c>
@@ -13905,8 +13901,8 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="149"/>
-      <c r="B50" s="147"/>
+      <c r="A50" s="152"/>
+      <c r="B50" s="153"/>
       <c r="C50" s="26" t="s">
         <v>968</v>
       </c>
@@ -13918,8 +13914,8 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="149"/>
-      <c r="B51" s="147"/>
+      <c r="A51" s="152"/>
+      <c r="B51" s="153"/>
       <c r="C51" s="26" t="s">
         <v>971</v>
       </c>
@@ -13931,8 +13927,8 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="149"/>
-      <c r="B52" s="147"/>
+      <c r="A52" s="152"/>
+      <c r="B52" s="153"/>
       <c r="C52" s="26" t="s">
         <v>974</v>
       </c>
@@ -13944,8 +13940,8 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="149"/>
-      <c r="B53" s="147"/>
+      <c r="A53" s="152"/>
+      <c r="B53" s="153"/>
       <c r="C53" s="26" t="s">
         <v>977</v>
       </c>
@@ -13957,8 +13953,8 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="149"/>
-      <c r="B54" s="147"/>
+      <c r="A54" s="152"/>
+      <c r="B54" s="153"/>
       <c r="C54" s="26" t="s">
         <v>979</v>
       </c>
@@ -13970,8 +13966,8 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="149"/>
-      <c r="B55" s="147"/>
+      <c r="A55" s="152"/>
+      <c r="B55" s="153"/>
       <c r="C55" s="26" t="s">
         <v>982</v>
       </c>
@@ -13983,10 +13979,10 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="149" t="s">
+      <c r="A56" s="152" t="s">
         <v>984</v>
       </c>
-      <c r="B56" s="147" t="s">
+      <c r="B56" s="153" t="s">
         <v>45</v>
       </c>
       <c r="C56" s="26" t="s">
@@ -14000,8 +13996,8 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="149"/>
-      <c r="B57" s="147"/>
+      <c r="A57" s="152"/>
+      <c r="B57" s="153"/>
       <c r="C57" s="28" t="s">
         <v>988</v>
       </c>
@@ -14013,8 +14009,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.8">
-      <c r="A58" s="149"/>
-      <c r="B58" s="147"/>
+      <c r="A58" s="152"/>
+      <c r="B58" s="153"/>
       <c r="C58" s="13" t="s">
         <v>991</v>
       </c>
@@ -14026,8 +14022,8 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="149"/>
-      <c r="B59" s="147"/>
+      <c r="A59" s="152"/>
+      <c r="B59" s="153"/>
       <c r="C59" s="28" t="s">
         <v>994</v>
       </c>
@@ -14039,8 +14035,8 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="149"/>
-      <c r="B60" s="147"/>
+      <c r="A60" s="152"/>
+      <c r="B60" s="153"/>
       <c r="C60" s="28" t="s">
         <v>997</v>
       </c>
@@ -14052,10 +14048,10 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="149" t="s">
+      <c r="A61" s="152" t="s">
         <v>1000</v>
       </c>
-      <c r="B61" s="147" t="s">
+      <c r="B61" s="153" t="s">
         <v>46</v>
       </c>
       <c r="C61" s="26" t="s">
@@ -14069,8 +14065,8 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="149"/>
-      <c r="B62" s="147"/>
+      <c r="A62" s="152"/>
+      <c r="B62" s="153"/>
       <c r="C62" s="26" t="s">
         <v>1004</v>
       </c>
@@ -14082,8 +14078,8 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="149"/>
-      <c r="B63" s="147"/>
+      <c r="A63" s="152"/>
+      <c r="B63" s="153"/>
       <c r="C63" s="26" t="s">
         <v>1007</v>
       </c>
@@ -14095,10 +14091,10 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="149" t="s">
+      <c r="A64" s="152" t="s">
         <v>1009</v>
       </c>
-      <c r="B64" s="147" t="s">
+      <c r="B64" s="153" t="s">
         <v>61</v>
       </c>
       <c r="C64" s="27" t="s">
@@ -14112,8 +14108,8 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="149"/>
-      <c r="B65" s="147"/>
+      <c r="A65" s="152"/>
+      <c r="B65" s="153"/>
       <c r="C65" s="26" t="s">
         <v>1013</v>
       </c>
@@ -14125,8 +14121,8 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="149"/>
-      <c r="B66" s="147"/>
+      <c r="A66" s="152"/>
+      <c r="B66" s="153"/>
       <c r="C66" s="26" t="s">
         <v>1016</v>
       </c>
@@ -14138,8 +14134,8 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="149"/>
-      <c r="B67" s="147"/>
+      <c r="A67" s="152"/>
+      <c r="B67" s="153"/>
       <c r="C67" s="26" t="s">
         <v>1019</v>
       </c>
@@ -14151,8 +14147,8 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="149"/>
-      <c r="B68" s="147"/>
+      <c r="A68" s="152"/>
+      <c r="B68" s="153"/>
       <c r="C68" s="26" t="s">
         <v>1022</v>
       </c>
@@ -14164,8 +14160,8 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="149"/>
-      <c r="B69" s="147"/>
+      <c r="A69" s="152"/>
+      <c r="B69" s="153"/>
       <c r="C69" s="26" t="s">
         <v>1025</v>
       </c>
@@ -14177,8 +14173,8 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="149"/>
-      <c r="B70" s="147"/>
+      <c r="A70" s="152"/>
+      <c r="B70" s="153"/>
       <c r="C70" s="26" t="s">
         <v>1028</v>
       </c>
@@ -14190,8 +14186,8 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="149"/>
-      <c r="B71" s="147"/>
+      <c r="A71" s="152"/>
+      <c r="B71" s="153"/>
       <c r="C71" s="26" t="s">
         <v>1031</v>
       </c>
@@ -14203,8 +14199,8 @@
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="149"/>
-      <c r="B72" s="147"/>
+      <c r="A72" s="152"/>
+      <c r="B72" s="153"/>
       <c r="C72" s="26" t="s">
         <v>1034</v>
       </c>
@@ -14216,10 +14212,10 @@
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="149" t="s">
+      <c r="A73" s="152" t="s">
         <v>1037</v>
       </c>
-      <c r="B73" s="147" t="s">
+      <c r="B73" s="153" t="s">
         <v>62</v>
       </c>
       <c r="C73" s="26" t="s">
@@ -14233,8 +14229,8 @@
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="149"/>
-      <c r="B74" s="147"/>
+      <c r="A74" s="152"/>
+      <c r="B74" s="153"/>
       <c r="C74" s="26" t="s">
         <v>1041</v>
       </c>
@@ -14246,8 +14242,8 @@
       </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="149"/>
-      <c r="B75" s="147"/>
+      <c r="A75" s="152"/>
+      <c r="B75" s="153"/>
       <c r="C75" s="26" t="s">
         <v>1044</v>
       </c>
@@ -14259,8 +14255,8 @@
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="149"/>
-      <c r="B76" s="147"/>
+      <c r="A76" s="152"/>
+      <c r="B76" s="153"/>
       <c r="C76" s="26" t="s">
         <v>1047</v>
       </c>
@@ -14272,21 +14268,21 @@
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="149" t="s">
+      <c r="A77" s="152" t="s">
         <v>1049</v>
       </c>
-      <c r="B77" s="147" t="s">
+      <c r="B77" s="153" t="s">
         <v>197</v>
       </c>
-      <c r="C77" s="153" t="s">
+      <c r="C77" s="148" t="s">
         <v>1748</v>
       </c>
-      <c r="D77" s="154"/>
-      <c r="E77" s="154"/>
+      <c r="D77" s="149"/>
+      <c r="E77" s="149"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="149"/>
-      <c r="B78" s="147"/>
+      <c r="A78" s="152"/>
+      <c r="B78" s="153"/>
       <c r="C78" s="58" t="s">
         <v>864</v>
       </c>
@@ -14298,8 +14294,8 @@
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="149"/>
-      <c r="B79" s="147"/>
+      <c r="A79" s="152"/>
+      <c r="B79" s="153"/>
       <c r="C79" s="58" t="s">
         <v>1722</v>
       </c>
@@ -14311,8 +14307,8 @@
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="149"/>
-      <c r="B80" s="147"/>
+      <c r="A80" s="152"/>
+      <c r="B80" s="153"/>
       <c r="C80" s="58" t="s">
         <v>1057</v>
       </c>
@@ -14324,8 +14320,8 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="149"/>
-      <c r="B81" s="147"/>
+      <c r="A81" s="152"/>
+      <c r="B81" s="153"/>
       <c r="C81" s="58" t="s">
         <v>861</v>
       </c>
@@ -14337,8 +14333,8 @@
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="149"/>
-      <c r="B82" s="147"/>
+      <c r="A82" s="152"/>
+      <c r="B82" s="153"/>
       <c r="C82" s="58" t="s">
         <v>854</v>
       </c>
@@ -14350,8 +14346,8 @@
       </c>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="149"/>
-      <c r="B83" s="147"/>
+      <c r="A83" s="152"/>
+      <c r="B83" s="153"/>
       <c r="C83" s="58" t="s">
         <v>1731</v>
       </c>
@@ -14363,8 +14359,8 @@
       </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="149"/>
-      <c r="B84" s="147"/>
+      <c r="A84" s="152"/>
+      <c r="B84" s="153"/>
       <c r="C84" s="58" t="s">
         <v>859</v>
       </c>
@@ -14376,8 +14372,8 @@
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="149"/>
-      <c r="B85" s="147"/>
+      <c r="A85" s="152"/>
+      <c r="B85" s="153"/>
       <c r="C85" s="58" t="s">
         <v>1736</v>
       </c>
@@ -14389,8 +14385,8 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="149"/>
-      <c r="B86" s="147"/>
+      <c r="A86" s="152"/>
+      <c r="B86" s="153"/>
       <c r="C86" s="58" t="s">
         <v>1739</v>
       </c>
@@ -14402,8 +14398,8 @@
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="149"/>
-      <c r="B87" s="147"/>
+      <c r="A87" s="152"/>
+      <c r="B87" s="153"/>
       <c r="C87" s="58" t="s">
         <v>1742</v>
       </c>
@@ -14415,8 +14411,8 @@
       </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="149"/>
-      <c r="B88" s="147"/>
+      <c r="A88" s="152"/>
+      <c r="B88" s="153"/>
       <c r="C88" s="58" t="s">
         <v>1745</v>
       </c>
@@ -14428,17 +14424,17 @@
       </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="149"/>
-      <c r="B89" s="147"/>
-      <c r="C89" s="153" t="s">
+      <c r="A89" s="152"/>
+      <c r="B89" s="153"/>
+      <c r="C89" s="148" t="s">
         <v>1749</v>
       </c>
-      <c r="D89" s="154"/>
-      <c r="E89" s="154"/>
+      <c r="D89" s="149"/>
+      <c r="E89" s="149"/>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="149"/>
-      <c r="B90" s="147"/>
+      <c r="A90" s="152"/>
+      <c r="B90" s="153"/>
       <c r="C90" s="26" t="s">
         <v>698</v>
       </c>
@@ -14450,8 +14446,8 @@
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="149"/>
-      <c r="B91" s="147"/>
+      <c r="A91" s="152"/>
+      <c r="B91" s="153"/>
       <c r="C91" s="26" t="s">
         <v>859</v>
       </c>
@@ -14463,8 +14459,8 @@
       </c>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="149"/>
-      <c r="B92" s="147"/>
+      <c r="A92" s="152"/>
+      <c r="B92" s="153"/>
       <c r="C92" s="26" t="s">
         <v>847</v>
       </c>
@@ -14476,8 +14472,8 @@
       </c>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="149"/>
-      <c r="B93" s="147"/>
+      <c r="A93" s="152"/>
+      <c r="B93" s="153"/>
       <c r="C93" s="26" t="s">
         <v>861</v>
       </c>
@@ -14489,8 +14485,8 @@
       </c>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="149"/>
-      <c r="B94" s="147"/>
+      <c r="A94" s="152"/>
+      <c r="B94" s="153"/>
       <c r="C94" s="26" t="s">
         <v>852</v>
       </c>
@@ -14502,8 +14498,8 @@
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="149"/>
-      <c r="B95" s="147"/>
+      <c r="A95" s="152"/>
+      <c r="B95" s="153"/>
       <c r="C95" s="26" t="s">
         <v>951</v>
       </c>
@@ -14515,8 +14511,8 @@
       </c>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="149"/>
-      <c r="B96" s="147"/>
+      <c r="A96" s="152"/>
+      <c r="B96" s="153"/>
       <c r="C96" s="26" t="s">
         <v>1057</v>
       </c>
@@ -14528,8 +14524,8 @@
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="149"/>
-      <c r="B97" s="147"/>
+      <c r="A97" s="152"/>
+      <c r="B97" s="153"/>
       <c r="C97" s="26" t="s">
         <v>1059</v>
       </c>
@@ -14541,10 +14537,10 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="149" t="s">
+      <c r="A98" s="152" t="s">
         <v>1060</v>
       </c>
-      <c r="B98" s="147" t="s">
+      <c r="B98" s="153" t="s">
         <v>49</v>
       </c>
       <c r="C98" s="26" t="s">
@@ -14558,8 +14554,8 @@
       </c>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="149"/>
-      <c r="B99" s="147"/>
+      <c r="A99" s="152"/>
+      <c r="B99" s="153"/>
       <c r="C99" s="26" t="s">
         <v>1064</v>
       </c>
@@ -14571,8 +14567,8 @@
       </c>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="149"/>
-      <c r="B100" s="147"/>
+      <c r="A100" s="152"/>
+      <c r="B100" s="153"/>
       <c r="C100" s="26" t="s">
         <v>1067</v>
       </c>
@@ -14584,10 +14580,10 @@
       </c>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="149" t="s">
+      <c r="A101" s="152" t="s">
         <v>1071</v>
       </c>
-      <c r="B101" s="147" t="s">
+      <c r="B101" s="153" t="s">
         <v>59</v>
       </c>
       <c r="C101" s="26" t="s">
@@ -14601,8 +14597,8 @@
       </c>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="149"/>
-      <c r="B102" s="147"/>
+      <c r="A102" s="152"/>
+      <c r="B102" s="153"/>
       <c r="C102" s="26" t="s">
         <v>1075</v>
       </c>
@@ -14614,8 +14610,8 @@
       </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="149"/>
-      <c r="B103" s="147"/>
+      <c r="A103" s="152"/>
+      <c r="B103" s="153"/>
       <c r="C103" s="26" t="s">
         <v>1078</v>
       </c>
@@ -14627,8 +14623,8 @@
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="149"/>
-      <c r="B104" s="147"/>
+      <c r="A104" s="152"/>
+      <c r="B104" s="153"/>
       <c r="C104" s="26" t="s">
         <v>1081</v>
       </c>
@@ -14640,10 +14636,10 @@
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="149" t="s">
+      <c r="A105" s="152" t="s">
         <v>1084</v>
       </c>
-      <c r="B105" s="147" t="s">
+      <c r="B105" s="153" t="s">
         <v>68</v>
       </c>
       <c r="C105" s="27" t="s">
@@ -14657,8 +14653,8 @@
       </c>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="149"/>
-      <c r="B106" s="147"/>
+      <c r="A106" s="152"/>
+      <c r="B106" s="153"/>
       <c r="C106" s="26" t="s">
         <v>1088</v>
       </c>
@@ -14670,10 +14666,10 @@
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="149" t="s">
+      <c r="A107" s="152" t="s">
         <v>1091</v>
       </c>
-      <c r="B107" s="147" t="s">
+      <c r="B107" s="153" t="s">
         <v>73</v>
       </c>
       <c r="C107" s="26" t="s">
@@ -14687,8 +14683,8 @@
       </c>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="149"/>
-      <c r="B108" s="147"/>
+      <c r="A108" s="152"/>
+      <c r="B108" s="153"/>
       <c r="C108" s="26" t="s">
         <v>1095</v>
       </c>
@@ -14700,10 +14696,10 @@
       </c>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="149" t="s">
+      <c r="A109" s="152" t="s">
         <v>1097</v>
       </c>
-      <c r="B109" s="147" t="s">
+      <c r="B109" s="153" t="s">
         <v>70</v>
       </c>
       <c r="C109" s="26" t="s">
@@ -14717,8 +14713,8 @@
       </c>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="149"/>
-      <c r="B110" s="147"/>
+      <c r="A110" s="152"/>
+      <c r="B110" s="153"/>
       <c r="C110" s="26" t="s">
         <v>1101</v>
       </c>
@@ -14730,8 +14726,8 @@
       </c>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="149"/>
-      <c r="B111" s="147"/>
+      <c r="A111" s="152"/>
+      <c r="B111" s="153"/>
       <c r="C111" s="26" t="s">
         <v>1103</v>
       </c>
@@ -14743,8 +14739,8 @@
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="149"/>
-      <c r="B112" s="147"/>
+      <c r="A112" s="152"/>
+      <c r="B112" s="153"/>
       <c r="C112" s="26" t="s">
         <v>1106</v>
       </c>
@@ -14756,10 +14752,10 @@
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="149" t="s">
+      <c r="A113" s="152" t="s">
         <v>1595</v>
       </c>
-      <c r="B113" s="147" t="s">
+      <c r="B113" s="153" t="s">
         <v>32</v>
       </c>
       <c r="C113" s="26" t="s">
@@ -14771,8 +14767,8 @@
       <c r="E113" s="26"/>
     </row>
     <row r="114" spans="1:6">
-      <c r="A114" s="149"/>
-      <c r="B114" s="147"/>
+      <c r="A114" s="152"/>
+      <c r="B114" s="153"/>
       <c r="C114" s="26" t="s">
         <v>1681</v>
       </c>
@@ -14782,8 +14778,8 @@
       <c r="E114" s="26"/>
     </row>
     <row r="115" spans="1:6">
-      <c r="A115" s="149"/>
-      <c r="B115" s="147"/>
+      <c r="A115" s="152"/>
+      <c r="B115" s="153"/>
       <c r="C115" s="124" t="s">
         <v>2140</v>
       </c>
@@ -14793,8 +14789,8 @@
       <c r="E115" s="26"/>
     </row>
     <row r="116" spans="1:6">
-      <c r="A116" s="149"/>
-      <c r="B116" s="147"/>
+      <c r="A116" s="152"/>
+      <c r="B116" s="153"/>
       <c r="C116" s="26" t="s">
         <v>1682</v>
       </c>
@@ -14804,8 +14800,8 @@
       <c r="E116" s="26"/>
     </row>
     <row r="117" spans="1:6">
-      <c r="A117" s="149"/>
-      <c r="B117" s="147"/>
+      <c r="A117" s="152"/>
+      <c r="B117" s="153"/>
       <c r="C117" s="26" t="s">
         <v>1683</v>
       </c>
@@ -14815,10 +14811,10 @@
       <c r="E117" s="26"/>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="149" t="s">
+      <c r="A118" s="152" t="s">
         <v>1597</v>
       </c>
-      <c r="B118" s="147" t="s">
+      <c r="B118" s="153" t="s">
         <v>34</v>
       </c>
       <c r="C118" s="26" t="s">
@@ -14830,8 +14826,8 @@
       <c r="E118" s="26"/>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="149"/>
-      <c r="B119" s="147"/>
+      <c r="A119" s="152"/>
+      <c r="B119" s="153"/>
       <c r="C119" s="26" t="s">
         <v>1689</v>
       </c>
@@ -14841,8 +14837,8 @@
       <c r="E119" s="26"/>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="149"/>
-      <c r="B120" s="147"/>
+      <c r="A120" s="152"/>
+      <c r="B120" s="153"/>
       <c r="C120" s="26" t="s">
         <v>1690</v>
       </c>
@@ -14852,10 +14848,10 @@
       <c r="E120" s="26"/>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="149" t="s">
+      <c r="A121" s="152" t="s">
         <v>1599</v>
       </c>
-      <c r="B121" s="147" t="s">
+      <c r="B121" s="153" t="s">
         <v>22</v>
       </c>
       <c r="C121" s="26" t="s">
@@ -14872,8 +14868,8 @@
       </c>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="149"/>
-      <c r="B122" s="147"/>
+      <c r="A122" s="152"/>
+      <c r="B122" s="153"/>
       <c r="C122" s="26" t="s">
         <v>1694</v>
       </c>
@@ -14888,8 +14884,8 @@
       </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="149"/>
-      <c r="B123" s="147"/>
+      <c r="A123" s="152"/>
+      <c r="B123" s="153"/>
       <c r="C123" s="26" t="s">
         <v>1695</v>
       </c>
@@ -14904,8 +14900,8 @@
       </c>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="149"/>
-      <c r="B124" s="147"/>
+      <c r="A124" s="152"/>
+      <c r="B124" s="153"/>
       <c r="C124" s="26" t="s">
         <v>1696</v>
       </c>
@@ -14920,8 +14916,8 @@
       </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="149"/>
-      <c r="B125" s="147"/>
+      <c r="A125" s="152"/>
+      <c r="B125" s="153"/>
       <c r="C125" s="26" t="s">
         <v>1697</v>
       </c>
@@ -14936,8 +14932,8 @@
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="149"/>
-      <c r="B126" s="147"/>
+      <c r="A126" s="152"/>
+      <c r="B126" s="153"/>
       <c r="C126" s="26" t="s">
         <v>1698</v>
       </c>
@@ -14952,8 +14948,8 @@
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="149"/>
-      <c r="B127" s="147"/>
+      <c r="A127" s="152"/>
+      <c r="B127" s="153"/>
       <c r="C127" s="13" t="s">
         <v>1699</v>
       </c>
@@ -14968,8 +14964,8 @@
       </c>
     </row>
     <row r="128" spans="1:6">
-      <c r="A128" s="149"/>
-      <c r="B128" s="147"/>
+      <c r="A128" s="152"/>
+      <c r="B128" s="153"/>
       <c r="C128" s="28" t="s">
         <v>1700</v>
       </c>
@@ -14984,8 +14980,8 @@
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" s="149"/>
-      <c r="B129" s="147"/>
+      <c r="A129" s="152"/>
+      <c r="B129" s="153"/>
       <c r="C129" s="28" t="s">
         <v>1701</v>
       </c>
@@ -15000,10 +14996,10 @@
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="A130" s="155">
+      <c r="A130" s="154">
         <v>25</v>
       </c>
-      <c r="B130" s="155" t="s">
+      <c r="B130" s="154" t="s">
         <v>1752</v>
       </c>
       <c r="C130" s="10" t="s">
@@ -15011,59 +15007,59 @@
       </c>
     </row>
     <row r="131" spans="1:6">
-      <c r="A131" s="145"/>
-      <c r="B131" s="145"/>
+      <c r="A131" s="146"/>
+      <c r="B131" s="146"/>
       <c r="C131" t="s">
         <v>1754</v>
       </c>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" s="145"/>
-      <c r="B132" s="145"/>
+      <c r="A132" s="146"/>
+      <c r="B132" s="146"/>
       <c r="C132" t="s">
         <v>1755</v>
       </c>
     </row>
     <row r="133" spans="1:6">
-      <c r="A133" s="145"/>
-      <c r="B133" s="145"/>
+      <c r="A133" s="146"/>
+      <c r="B133" s="146"/>
       <c r="C133" t="s">
         <v>1756</v>
       </c>
     </row>
     <row r="134" spans="1:6">
-      <c r="A134" s="145"/>
-      <c r="B134" s="145"/>
+      <c r="A134" s="146"/>
+      <c r="B134" s="146"/>
       <c r="C134" t="s">
         <v>1757</v>
       </c>
     </row>
     <row r="135" spans="1:6">
-      <c r="A135" s="145"/>
-      <c r="B135" s="145"/>
+      <c r="A135" s="146"/>
+      <c r="B135" s="146"/>
       <c r="C135" t="s">
         <v>1758</v>
       </c>
     </row>
     <row r="136" spans="1:6">
-      <c r="A136" s="145"/>
-      <c r="B136" s="145"/>
+      <c r="A136" s="146"/>
+      <c r="B136" s="146"/>
       <c r="C136" t="s">
         <v>1759</v>
       </c>
     </row>
     <row r="137" spans="1:6">
-      <c r="A137" s="145"/>
-      <c r="B137" s="145"/>
+      <c r="A137" s="146"/>
+      <c r="B137" s="146"/>
       <c r="C137" t="s">
         <v>1760</v>
       </c>
     </row>
     <row r="138" spans="1:6">
-      <c r="A138" s="145">
+      <c r="A138" s="146">
         <v>26</v>
       </c>
-      <c r="B138" s="146" t="s">
+      <c r="B138" s="147" t="s">
         <v>1761</v>
       </c>
       <c r="C138" s="13" t="s">
@@ -15074,8 +15070,8 @@
       </c>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" s="145"/>
-      <c r="B139" s="146"/>
+      <c r="A139" s="146"/>
+      <c r="B139" s="147"/>
       <c r="C139" s="13" t="s">
         <v>1764</v>
       </c>
@@ -15084,8 +15080,8 @@
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="145"/>
-      <c r="B140" s="146"/>
+      <c r="A140" s="146"/>
+      <c r="B140" s="147"/>
       <c r="C140" s="13" t="s">
         <v>1047</v>
       </c>
@@ -15094,10 +15090,10 @@
       </c>
     </row>
     <row r="141" spans="1:6">
-      <c r="A141" s="145">
+      <c r="A141" s="146">
         <v>27</v>
       </c>
-      <c r="B141" s="146" t="s">
+      <c r="B141" s="147" t="s">
         <v>1791</v>
       </c>
       <c r="C141" s="13" t="s">
@@ -15111,8 +15107,8 @@
       </c>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="145"/>
-      <c r="B142" s="146"/>
+      <c r="A142" s="146"/>
+      <c r="B142" s="147"/>
       <c r="C142" s="13" t="s">
         <v>1769</v>
       </c>
@@ -15124,8 +15120,8 @@
       </c>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="145"/>
-      <c r="B143" s="146"/>
+      <c r="A143" s="146"/>
+      <c r="B143" s="147"/>
       <c r="C143" s="13" t="s">
         <v>1772</v>
       </c>
@@ -15137,8 +15133,8 @@
       </c>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="145"/>
-      <c r="B144" s="146"/>
+      <c r="A144" s="146"/>
+      <c r="B144" s="147"/>
       <c r="C144" s="13" t="s">
         <v>1775</v>
       </c>
@@ -15150,8 +15146,8 @@
       </c>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="145"/>
-      <c r="B145" s="146"/>
+      <c r="A145" s="146"/>
+      <c r="B145" s="147"/>
       <c r="C145" s="13" t="s">
         <v>1778</v>
       </c>
@@ -15163,8 +15159,8 @@
       </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="145"/>
-      <c r="B146" s="146"/>
+      <c r="A146" s="146"/>
+      <c r="B146" s="147"/>
       <c r="C146" s="13" t="s">
         <v>1781</v>
       </c>
@@ -15176,8 +15172,8 @@
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="145"/>
-      <c r="B147" s="146"/>
+      <c r="A147" s="146"/>
+      <c r="B147" s="147"/>
       <c r="C147" s="13" t="s">
         <v>1784</v>
       </c>
@@ -15189,8 +15185,8 @@
       </c>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="145"/>
-      <c r="B148" s="146"/>
+      <c r="A148" s="146"/>
+      <c r="B148" s="147"/>
       <c r="C148" s="13" t="s">
         <v>1787</v>
       </c>
@@ -15202,8 +15198,8 @@
       </c>
     </row>
     <row r="149" spans="1:5" ht="28.8">
-      <c r="A149" s="145"/>
-      <c r="B149" s="146"/>
+      <c r="A149" s="146"/>
+      <c r="B149" s="147"/>
       <c r="C149" s="13" t="s">
         <v>845</v>
       </c>
@@ -15215,44 +15211,44 @@
       </c>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="145">
+      <c r="A150" s="146">
         <v>28</v>
       </c>
-      <c r="B150" s="157" t="s">
+      <c r="B150" s="151" t="s">
         <v>196</v>
       </c>
-      <c r="C150" s="153" t="s">
+      <c r="C150" s="148" t="s">
         <v>1749</v>
       </c>
-      <c r="D150" s="154"/>
-      <c r="E150" s="154"/>
+      <c r="D150" s="149"/>
+      <c r="E150" s="149"/>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="145"/>
-      <c r="B151" s="157"/>
-      <c r="C151" s="156" t="s">
+      <c r="A151" s="146"/>
+      <c r="B151" s="151"/>
+      <c r="C151" s="150" t="s">
         <v>1799</v>
       </c>
-      <c r="D151" s="156"/>
-      <c r="E151" s="156"/>
+      <c r="D151" s="150"/>
+      <c r="E151" s="150"/>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="145"/>
-      <c r="B152" s="157"/>
-      <c r="C152" s="153" t="s">
+      <c r="A152" s="146"/>
+      <c r="B152" s="151"/>
+      <c r="C152" s="148" t="s">
         <v>1748</v>
       </c>
-      <c r="D152" s="154"/>
-      <c r="E152" s="154"/>
+      <c r="D152" s="149"/>
+      <c r="E152" s="149"/>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="145"/>
-      <c r="B153" s="157"/>
-      <c r="C153" s="156" t="s">
+      <c r="A153" s="146"/>
+      <c r="B153" s="151"/>
+      <c r="C153" s="150" t="s">
         <v>1800</v>
       </c>
-      <c r="D153" s="156"/>
-      <c r="E153" s="156"/>
+      <c r="D153" s="150"/>
+      <c r="E153" s="150"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="56">
@@ -15272,7 +15268,7 @@
       <c r="A155" s="56">
         <v>30</v>
       </c>
-      <c r="B155" s="146" t="s">
+      <c r="B155" s="147" t="s">
         <v>42</v>
       </c>
       <c r="C155" s="80" t="s">
@@ -15286,7 +15282,7 @@
       </c>
     </row>
     <row r="156" spans="1:5">
-      <c r="B156" s="146"/>
+      <c r="B156" s="147"/>
       <c r="C156" s="80" t="s">
         <v>1839</v>
       </c>
@@ -15298,7 +15294,7 @@
       </c>
     </row>
     <row r="157" spans="1:5" ht="28.8">
-      <c r="B157" s="146"/>
+      <c r="B157" s="147"/>
       <c r="C157" s="80" t="s">
         <v>1841</v>
       </c>
@@ -15310,7 +15306,7 @@
       </c>
     </row>
     <row r="158" spans="1:5" ht="43.2">
-      <c r="B158" s="146"/>
+      <c r="B158" s="147"/>
       <c r="C158" s="80" t="s">
         <v>1844</v>
       </c>
@@ -15321,8 +15317,8 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="43.2">
-      <c r="B159" s="146"/>
+    <row r="159" spans="1:5" ht="28.8">
+      <c r="B159" s="147"/>
       <c r="C159" s="80" t="s">
         <v>1847</v>
       </c>
@@ -15334,7 +15330,7 @@
       </c>
     </row>
     <row r="160" spans="1:5" ht="43.2">
-      <c r="B160" s="146"/>
+      <c r="B160" s="147"/>
       <c r="C160" s="80" t="s">
         <v>1850</v>
       </c>
@@ -15346,7 +15342,7 @@
       </c>
     </row>
     <row r="161" spans="1:5" ht="28.8">
-      <c r="B161" s="146"/>
+      <c r="B161" s="147"/>
       <c r="C161" s="80" t="s">
         <v>1853</v>
       </c>
@@ -15358,7 +15354,7 @@
       </c>
     </row>
     <row r="162" spans="1:5" ht="28.8">
-      <c r="B162" s="146"/>
+      <c r="B162" s="147"/>
       <c r="C162" s="80" t="s">
         <v>1856</v>
       </c>
@@ -15370,7 +15366,7 @@
       </c>
     </row>
     <row r="163" spans="1:5" ht="28.8">
-      <c r="B163" s="146"/>
+      <c r="B163" s="147"/>
       <c r="C163" s="80" t="s">
         <v>1859</v>
       </c>
@@ -15382,7 +15378,7 @@
       </c>
     </row>
     <row r="164" spans="1:5" ht="28.8">
-      <c r="B164" s="146"/>
+      <c r="B164" s="147"/>
       <c r="C164" s="80" t="s">
         <v>1862</v>
       </c>
@@ -15394,7 +15390,7 @@
       </c>
     </row>
     <row r="165" spans="1:5" ht="28.8">
-      <c r="B165" s="146"/>
+      <c r="B165" s="147"/>
       <c r="C165" s="80" t="s">
         <v>1865</v>
       </c>
@@ -15406,7 +15402,7 @@
       </c>
     </row>
     <row r="166" spans="1:5" ht="28.8">
-      <c r="B166" s="146"/>
+      <c r="B166" s="147"/>
       <c r="C166" s="80" t="s">
         <v>1868</v>
       </c>
@@ -15417,8 +15413,8 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="28.8">
-      <c r="B167" s="146"/>
+    <row r="167" spans="1:5">
+      <c r="B167" s="147"/>
       <c r="C167" s="80" t="s">
         <v>1871</v>
       </c>
@@ -15430,7 +15426,7 @@
       </c>
     </row>
     <row r="168" spans="1:5">
-      <c r="B168" s="146"/>
+      <c r="B168" s="147"/>
       <c r="C168" s="80" t="s">
         <v>1874</v>
       </c>
@@ -15445,7 +15441,7 @@
       <c r="A169" s="56">
         <v>31</v>
       </c>
-      <c r="B169" s="146" t="s">
+      <c r="B169" s="147" t="s">
         <v>1935</v>
       </c>
       <c r="C169" s="87" t="s">
@@ -15454,16 +15450,16 @@
       <c r="D169" s="88"/>
     </row>
     <row r="170" spans="1:5">
-      <c r="B170" s="146"/>
+      <c r="B170" s="147"/>
       <c r="C170" s="87" t="s">
         <v>1938</v>
       </c>
     </row>
     <row r="171" spans="1:5">
-      <c r="A171" s="145">
+      <c r="A171" s="146">
         <v>32</v>
       </c>
-      <c r="B171" s="146" t="s">
+      <c r="B171" s="147" t="s">
         <v>2136</v>
       </c>
       <c r="C171" s="87" t="s">
@@ -15471,197 +15467,225 @@
       </c>
     </row>
     <row r="172" spans="1:5">
-      <c r="A172" s="145"/>
-      <c r="B172" s="146"/>
+      <c r="A172" s="146"/>
+      <c r="B172" s="147"/>
       <c r="C172" s="87" t="s">
         <v>2138</v>
       </c>
     </row>
     <row r="173" spans="1:5">
-      <c r="A173" s="145"/>
-      <c r="B173" s="146"/>
+      <c r="A173" s="146"/>
+      <c r="B173" s="147"/>
       <c r="C173" s="87" t="s">
         <v>2139</v>
       </c>
     </row>
     <row r="174" spans="1:5">
-      <c r="A174" s="143">
+      <c r="A174" s="138">
         <v>34</v>
       </c>
-      <c r="B174" s="138" t="s">
+      <c r="B174" s="159" t="s">
+        <v>2194</v>
+      </c>
+      <c r="C174" s="139" t="s">
+        <v>2183</v>
+      </c>
+      <c r="D174" s="140" t="s">
+        <v>2183</v>
+      </c>
+      <c r="E174" s="141" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="138"/>
+      <c r="B175" s="159"/>
+      <c r="C175" s="139" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D175" s="140" t="s">
+        <v>2196</v>
+      </c>
+      <c r="E175" s="139" t="s">
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="138"/>
+      <c r="B176" s="159"/>
+      <c r="C176" s="139" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D176" s="140" t="s">
+        <v>2198</v>
+      </c>
+      <c r="E176" s="139" t="s">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="138"/>
+      <c r="B177" s="159"/>
+      <c r="C177" s="139" t="s">
+        <v>2200</v>
+      </c>
+      <c r="D177" s="140" t="s">
+        <v>2201</v>
+      </c>
+      <c r="E177" s="139" t="s">
         <v>2202</v>
       </c>
-      <c r="C174" s="163" t="s">
-        <v>2184</v>
-      </c>
-      <c r="D174" s="164" t="s">
-        <v>2184</v>
-      </c>
-      <c r="E174" s="165" t="s">
+    </row>
+    <row r="178" spans="1:6" ht="28.8">
+      <c r="A178" s="138"/>
+      <c r="B178" s="159"/>
+      <c r="C178" s="139" t="s">
         <v>2203</v>
       </c>
-    </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="143"/>
-      <c r="B175" s="138"/>
-      <c r="C175" s="163" t="s">
-        <v>2181</v>
-      </c>
-      <c r="D175" s="164" t="s">
+      <c r="D178" s="140" t="s">
         <v>2204</v>
       </c>
-      <c r="E175" s="163" t="s">
+      <c r="E178" s="139" t="s">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="138"/>
+      <c r="B179" s="159"/>
+      <c r="C179" s="139" t="s">
+        <v>2182</v>
+      </c>
+      <c r="D179" s="140" t="s">
+        <v>2182</v>
+      </c>
+      <c r="E179" s="139" t="s">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="138"/>
+      <c r="B180" s="159"/>
+      <c r="C180" s="139" t="s">
         <v>2205</v>
       </c>
-    </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="143"/>
-      <c r="B176" s="138"/>
-      <c r="C176" s="163" t="s">
-        <v>2182</v>
-      </c>
-      <c r="D176" s="164" t="s">
+      <c r="D180" s="140" t="s">
+        <v>2205</v>
+      </c>
+      <c r="E180" s="139" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="B181" s="159"/>
+      <c r="C181" s="139" t="s">
         <v>2206</v>
       </c>
-      <c r="E176" s="163" t="s">
+      <c r="D181" s="140" t="s">
         <v>2207</v>
       </c>
-    </row>
-    <row r="177" spans="1:6">
-      <c r="A177" s="143"/>
-      <c r="B177" s="138"/>
-      <c r="C177" s="163" t="s">
-        <v>2208</v>
-      </c>
-      <c r="D177" s="164" t="s">
-        <v>2209</v>
-      </c>
-      <c r="E177" s="163" t="s">
-        <v>2210</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" ht="28.8">
-      <c r="A178" s="143"/>
-      <c r="B178" s="138"/>
-      <c r="C178" s="163" t="s">
-        <v>2211</v>
-      </c>
-      <c r="D178" s="164" t="s">
-        <v>2212</v>
-      </c>
-      <c r="E178" s="163" t="s">
-        <v>2212</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
-      <c r="A179" s="143"/>
-      <c r="B179" s="138"/>
-      <c r="C179" s="163" t="s">
-        <v>2183</v>
-      </c>
-      <c r="D179" s="164" t="s">
-        <v>2183</v>
-      </c>
-      <c r="E179" s="163" t="s">
-        <v>2183</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
-      <c r="A180" s="143"/>
-      <c r="B180" s="138"/>
-      <c r="C180" s="163" t="s">
-        <v>2213</v>
-      </c>
-      <c r="D180" s="164" t="s">
-        <v>2213</v>
-      </c>
-      <c r="E180" s="163" t="s">
-        <v>2213</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6">
-      <c r="B181" s="138"/>
-      <c r="C181" s="163" t="s">
-        <v>2214</v>
-      </c>
-      <c r="D181" s="164" t="s">
-        <v>2215</v>
-      </c>
-      <c r="E181" s="163" t="s">
-        <v>2215</v>
-      </c>
-      <c r="F181" s="163"/>
+      <c r="E181" s="139" t="s">
+        <v>2207</v>
+      </c>
+      <c r="F181" s="139"/>
     </row>
     <row r="182" spans="1:6" ht="28.8">
       <c r="A182" s="56">
         <v>35</v>
       </c>
-      <c r="B182" s="166" t="s">
-        <v>2199</v>
-      </c>
-      <c r="C182" s="163" t="s">
-        <v>2216</v>
-      </c>
-      <c r="D182" s="164" t="s">
-        <v>2217</v>
-      </c>
-      <c r="E182" s="165" t="s">
-        <v>2217</v>
+      <c r="B182" s="159" t="s">
+        <v>2223</v>
+      </c>
+      <c r="C182" s="139" t="s">
+        <v>2208</v>
+      </c>
+      <c r="D182" s="140" t="s">
+        <v>2209</v>
+      </c>
+      <c r="E182" s="141" t="s">
+        <v>2209</v>
       </c>
     </row>
     <row r="183" spans="1:6">
-      <c r="B183" s="166"/>
-      <c r="C183" s="163" t="s">
-        <v>2218</v>
-      </c>
-      <c r="D183" s="164" t="s">
-        <v>2219</v>
-      </c>
-      <c r="E183" s="163" t="s">
-        <v>2219</v>
+      <c r="B183" s="159"/>
+      <c r="C183" s="139" t="s">
+        <v>2210</v>
+      </c>
+      <c r="D183" s="140" t="s">
+        <v>2211</v>
+      </c>
+      <c r="E183" s="139" t="s">
+        <v>2211</v>
       </c>
     </row>
     <row r="184" spans="1:6">
-      <c r="B184" s="166"/>
-      <c r="C184" s="163" t="s">
-        <v>2214</v>
-      </c>
-      <c r="D184" s="164" t="s">
-        <v>2215</v>
-      </c>
-      <c r="E184" s="163" t="s">
-        <v>2215</v>
+      <c r="B184" s="159"/>
+      <c r="C184" s="139" t="s">
+        <v>2206</v>
+      </c>
+      <c r="D184" s="140" t="s">
+        <v>2207</v>
+      </c>
+      <c r="E184" s="139" t="s">
+        <v>2207</v>
       </c>
     </row>
     <row r="185" spans="1:6">
-      <c r="B185" s="166" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C185" s="163" t="s">
+      <c r="B185" s="159"/>
+      <c r="C185" s="139" t="s">
         <v>1874</v>
       </c>
-      <c r="D185" s="164" t="s">
-        <v>2221</v>
-      </c>
-      <c r="E185" s="163" t="s">
-        <v>2220</v>
+      <c r="D185" s="140" t="s">
+        <v>2213</v>
+      </c>
+      <c r="E185" s="139" t="s">
+        <v>2212</v>
       </c>
     </row>
     <row r="189" spans="1:6">
-      <c r="F189" s="163"/>
+      <c r="F189" s="139"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="B171:B173"/>
-    <mergeCell ref="A171:A173"/>
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="A150:A153"/>
-    <mergeCell ref="B155:B168"/>
-    <mergeCell ref="C150:E150"/>
-    <mergeCell ref="C151:E151"/>
-    <mergeCell ref="C152:E152"/>
-    <mergeCell ref="C153:E153"/>
-    <mergeCell ref="B150:B153"/>
+  <mergeCells count="66">
+    <mergeCell ref="B174:B181"/>
+    <mergeCell ref="B182:B185"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B141:B149"/>
+    <mergeCell ref="A141:A149"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A45:A55"/>
+    <mergeCell ref="B45:B55"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="A64:A72"/>
+    <mergeCell ref="B64:B72"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="A77:A97"/>
+    <mergeCell ref="B77:B97"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="A109:A112"/>
+    <mergeCell ref="B109:B112"/>
     <mergeCell ref="B138:B140"/>
     <mergeCell ref="A138:A140"/>
     <mergeCell ref="C77:E77"/>
@@ -15676,46 +15700,18 @@
     <mergeCell ref="B101:B104"/>
     <mergeCell ref="B130:B137"/>
     <mergeCell ref="A130:A137"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="A77:A97"/>
-    <mergeCell ref="B77:B97"/>
     <mergeCell ref="A121:A129"/>
     <mergeCell ref="B121:B129"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="A109:A112"/>
-    <mergeCell ref="B109:B112"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A64:A72"/>
-    <mergeCell ref="B64:B72"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B141:B149"/>
-    <mergeCell ref="A141:A149"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A45:A55"/>
-    <mergeCell ref="B45:B55"/>
+    <mergeCell ref="C150:E150"/>
+    <mergeCell ref="C151:E151"/>
+    <mergeCell ref="C152:E152"/>
+    <mergeCell ref="C153:E153"/>
+    <mergeCell ref="B150:B153"/>
+    <mergeCell ref="B171:B173"/>
+    <mergeCell ref="A171:A173"/>
+    <mergeCell ref="B169:B170"/>
+    <mergeCell ref="A150:A153"/>
+    <mergeCell ref="B155:B168"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15766,7 +15762,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="160" t="s">
         <v>119</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -15789,7 +15785,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8">
-      <c r="A3" s="157"/>
+      <c r="A3" s="151"/>
       <c r="B3" s="63" t="s">
         <v>129</v>
       </c>
@@ -15810,7 +15806,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="157"/>
+      <c r="A4" s="151"/>
       <c r="B4" s="63" t="s">
         <v>132</v>
       </c>
@@ -15831,7 +15827,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="130" customFormat="1" ht="28.8">
-      <c r="A5" s="157"/>
+      <c r="A5" s="151"/>
       <c r="B5" s="127" t="s">
         <v>135</v>
       </c>
@@ -15852,7 +15848,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="157"/>
+      <c r="A6" s="151"/>
       <c r="B6" s="63" t="s">
         <v>137</v>
       </c>
@@ -15873,7 +15869,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8">
-      <c r="A7" s="157"/>
+      <c r="A7" s="151"/>
       <c r="B7" s="63" t="s">
         <v>140</v>
       </c>
@@ -15894,7 +15890,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2">
-      <c r="A8" s="157"/>
+      <c r="A8" s="151"/>
       <c r="B8" s="66" t="s">
         <v>142</v>
       </c>
@@ -15915,7 +15911,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8">
-      <c r="A9" s="157"/>
+      <c r="A9" s="151"/>
       <c r="B9" s="66" t="s">
         <v>144</v>
       </c>
@@ -15936,7 +15932,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A10" s="157"/>
+      <c r="A10" s="151"/>
       <c r="B10" s="74" t="s">
         <v>145</v>
       </c>
@@ -15957,7 +15953,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A11" s="157"/>
+      <c r="A11" s="151"/>
       <c r="B11" s="74" t="s">
         <v>146</v>
       </c>
@@ -15978,7 +15974,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A12" s="157"/>
+      <c r="A12" s="151"/>
       <c r="B12" s="74" t="s">
         <v>148</v>
       </c>
@@ -15999,7 +15995,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A13" s="157"/>
+      <c r="A13" s="151"/>
       <c r="B13" s="74" t="s">
         <v>150</v>
       </c>
@@ -16020,7 +16016,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.2">
-      <c r="A14" s="157"/>
+      <c r="A14" s="151"/>
       <c r="B14" s="66" t="s">
         <v>151</v>
       </c>
@@ -16041,7 +16037,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.2">
-      <c r="A15" s="157"/>
+      <c r="A15" s="151"/>
       <c r="B15" s="66" t="s">
         <v>154</v>
       </c>
@@ -16062,7 +16058,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A16" s="157"/>
+      <c r="A16" s="151"/>
       <c r="B16" s="66" t="s">
         <v>156</v>
       </c>
@@ -16083,7 +16079,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="100.8">
-      <c r="A17" s="157"/>
+      <c r="A17" s="151"/>
       <c r="B17" s="66" t="s">
         <v>158</v>
       </c>
@@ -18991,7 +18987,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="40" t="s">
-        <v>2189</v>
+        <v>2187</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>837</v>
@@ -21232,15 +21228,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000CEFFC18343FB94BABD97DFE0FB52C36" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e9249330997f821dfdee74745ca5f75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa0a58a8-6aee-41ea-a8cf-318e5bdc9d94" xmlns:ns3="bce336b2-2120-40dd-bb83-70ede1f6399d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f22989ebbefe26683b07a60ab4551e6d" ns2:_="" ns3:_="">
     <xsd:import namespace="fa0a58a8-6aee-41ea-a8cf-318e5bdc9d94"/>
@@ -21437,6 +21424,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -21444,14 +21440,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F835A65A-8852-436B-8C93-990B831CCA81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09A7D9CE-337B-4411-B4CC-E126096FC6FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21466,6 +21454,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F835A65A-8852-436B-8C93-990B831CCA81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
prescription spelling in update
</commit_message>
<xml_diff>
--- a/Nphies-GapSheetV2.8.xlsx
+++ b/Nphies-GapSheetV2.8.xlsx
@@ -7162,9 +7162,6 @@
     <t xml:space="preserve">Others : specify </t>
   </si>
   <si>
-    <t>Added NPHIES_CLAIMINFO -&gt; PRESCRPTION</t>
-  </si>
-  <si>
     <t>Added NPHIES_CLAIMITEM -&gt; PHARMACISTSELECTIONREASON</t>
   </si>
   <si>
@@ -7223,6 +7220,9 @@
   </si>
   <si>
     <t>Added NPHIES_CLAIMITEM -&gt; PRESCIBEDDRUGCODE</t>
+  </si>
+  <si>
+    <t>Added NPHIES_CLAIMINFO -&gt; PRESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -8170,28 +8170,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8203,11 +8194,20 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8588,7 +8588,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8794,54 +8794,54 @@
         <v>2.8</v>
       </c>
       <c r="B33" t="s">
-        <v>2214</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="B34" s="10" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="B35" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="B37" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="138"/>
       <c r="B38" s="10" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="C38" s="138"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="138"/>
       <c r="B39" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="C39" s="138"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="138"/>
       <c r="B40" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="C40" s="138"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="138"/>
       <c r="B41" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="C41" s="138"/>
     </row>
@@ -10445,7 +10445,7 @@
   <dimension ref="A1:H199"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
@@ -11345,7 +11345,7 @@
     </row>
     <row r="65" spans="1:8" s="142" customFormat="1">
       <c r="B65" s="142" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
       <c r="C65" s="142" t="s">
         <v>77</v>
@@ -11354,7 +11354,7 @@
         <v>31</v>
       </c>
       <c r="E65" s="144" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -11688,7 +11688,7 @@
     </row>
     <row r="90" spans="1:8" ht="28.8">
       <c r="B90" s="21" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="C90" t="s">
         <v>77</v>
@@ -11704,7 +11704,7 @@
     </row>
     <row r="91" spans="1:8">
       <c r="B91" s="20" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="C91" t="s">
         <v>77</v>
@@ -11748,7 +11748,7 @@
     </row>
     <row r="94" spans="1:8" s="142" customFormat="1">
       <c r="B94" s="142" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="C94" s="142" t="s">
         <v>77</v>
@@ -11757,7 +11757,7 @@
         <v>31</v>
       </c>
       <c r="E94" s="142" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="H94" s="143"/>
     </row>
@@ -11984,12 +11984,12 @@
         <v>72</v>
       </c>
       <c r="E110" s="142" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="111" spans="2:8" s="142" customFormat="1">
       <c r="B111" s="142" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="C111" s="142" t="s">
         <v>78</v>
@@ -11998,12 +11998,12 @@
         <v>31</v>
       </c>
       <c r="E111" s="142" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="112" spans="2:8" s="142" customFormat="1">
       <c r="B112" s="142" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="C112" s="142" t="s">
         <v>77</v>
@@ -12012,7 +12012,7 @@
         <v>31</v>
       </c>
       <c r="E112" s="142" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="H112" s="144"/>
     </row>
@@ -12084,7 +12084,7 @@
     </row>
     <row r="118" spans="1:8">
       <c r="B118" s="21" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="C118" t="s">
         <v>77</v>
@@ -12100,7 +12100,7 @@
     </row>
     <row r="119" spans="1:8">
       <c r="B119" s="20" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="C119" t="s">
         <v>77</v>
@@ -12233,12 +12233,12 @@
         <v>72</v>
       </c>
       <c r="E128" s="142" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="142" customFormat="1">
       <c r="B129" s="142" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="C129" s="142" t="s">
         <v>78</v>
@@ -12247,12 +12247,12 @@
         <v>31</v>
       </c>
       <c r="E129" s="142" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="130" spans="1:8" s="142" customFormat="1">
       <c r="B130" s="142" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="C130" s="142" t="s">
         <v>77</v>
@@ -12261,12 +12261,12 @@
         <v>31</v>
       </c>
       <c r="E130" s="142" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="131" spans="1:8" s="142" customFormat="1">
       <c r="B131" s="142" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="C131" s="142" t="s">
         <v>77</v>
@@ -12275,7 +12275,7 @@
         <v>31</v>
       </c>
       <c r="E131" s="142" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="H131" s="143"/>
     </row>
@@ -13243,10 +13243,10 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="147">
+      <c r="A2" s="148">
         <v>1</v>
       </c>
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="152" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -13260,8 +13260,8 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="147"/>
-      <c r="B3" s="153"/>
+      <c r="A3" s="148"/>
+      <c r="B3" s="149"/>
       <c r="C3" s="26" t="s">
         <v>842</v>
       </c>
@@ -13273,8 +13273,8 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="147"/>
-      <c r="B4" s="153"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="149"/>
       <c r="C4" s="26" t="s">
         <v>845</v>
       </c>
@@ -13286,8 +13286,8 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="147"/>
-      <c r="B5" s="153"/>
+      <c r="A5" s="148"/>
+      <c r="B5" s="149"/>
       <c r="C5" s="26" t="s">
         <v>847</v>
       </c>
@@ -13299,8 +13299,8 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="147"/>
-      <c r="B6" s="153"/>
+      <c r="A6" s="148"/>
+      <c r="B6" s="149"/>
       <c r="C6" s="26" t="s">
         <v>850</v>
       </c>
@@ -13312,8 +13312,8 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="147"/>
-      <c r="B7" s="153"/>
+      <c r="A7" s="148"/>
+      <c r="B7" s="149"/>
       <c r="C7" s="26" t="s">
         <v>852</v>
       </c>
@@ -13325,8 +13325,8 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="147"/>
-      <c r="B8" s="153"/>
+      <c r="A8" s="148"/>
+      <c r="B8" s="149"/>
       <c r="C8" s="26" t="s">
         <v>854</v>
       </c>
@@ -13338,8 +13338,8 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="147"/>
-      <c r="B9" s="153"/>
+      <c r="A9" s="148"/>
+      <c r="B9" s="149"/>
       <c r="C9" s="26" t="s">
         <v>856</v>
       </c>
@@ -13351,10 +13351,10 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="152" t="s">
+      <c r="A10" s="150" t="s">
         <v>858</v>
       </c>
-      <c r="B10" s="153" t="s">
+      <c r="B10" s="149" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="26" t="s">
@@ -13368,8 +13368,8 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="152"/>
-      <c r="B11" s="153"/>
+      <c r="A11" s="150"/>
+      <c r="B11" s="149"/>
       <c r="C11" s="26" t="s">
         <v>861</v>
       </c>
@@ -13381,8 +13381,8 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="152"/>
-      <c r="B12" s="153"/>
+      <c r="A12" s="150"/>
+      <c r="B12" s="149"/>
       <c r="C12" s="26" t="s">
         <v>864</v>
       </c>
@@ -13394,8 +13394,8 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="152"/>
-      <c r="B13" s="153"/>
+      <c r="A13" s="150"/>
+      <c r="B13" s="149"/>
       <c r="C13" s="26" t="s">
         <v>847</v>
       </c>
@@ -13407,8 +13407,8 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="152"/>
-      <c r="B14" s="153"/>
+      <c r="A14" s="150"/>
+      <c r="B14" s="149"/>
       <c r="C14" s="26" t="s">
         <v>869</v>
       </c>
@@ -13420,10 +13420,10 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="152" t="s">
+      <c r="A15" s="150" t="s">
         <v>872</v>
       </c>
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="153" t="s">
         <v>873</v>
       </c>
       <c r="C15" s="26" t="s">
@@ -13437,8 +13437,8 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="152"/>
-      <c r="B16" s="157"/>
+      <c r="A16" s="150"/>
+      <c r="B16" s="154"/>
       <c r="C16" s="26" t="s">
         <v>877</v>
       </c>
@@ -13450,8 +13450,8 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="152"/>
-      <c r="B17" s="157"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="154"/>
       <c r="C17" s="26" t="s">
         <v>880</v>
       </c>
@@ -13463,8 +13463,8 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="152"/>
-      <c r="B18" s="157"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="154"/>
       <c r="C18" s="26" t="s">
         <v>883</v>
       </c>
@@ -13476,8 +13476,8 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="152"/>
-      <c r="B19" s="157"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="154"/>
       <c r="C19" s="26" t="s">
         <v>886</v>
       </c>
@@ -13489,8 +13489,8 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="152"/>
-      <c r="B20" s="157"/>
+      <c r="A20" s="150"/>
+      <c r="B20" s="154"/>
       <c r="C20" s="26" t="s">
         <v>889</v>
       </c>
@@ -13502,8 +13502,8 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="152"/>
-      <c r="B21" s="155"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="152"/>
       <c r="C21" s="26" t="s">
         <v>892</v>
       </c>
@@ -13515,10 +13515,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.8">
-      <c r="A22" s="158">
+      <c r="A22" s="151">
         <v>4</v>
       </c>
-      <c r="B22" s="153" t="s">
+      <c r="B22" s="149" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="27" t="s">
@@ -13532,8 +13532,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.2">
-      <c r="A23" s="147"/>
-      <c r="B23" s="153"/>
+      <c r="A23" s="148"/>
+      <c r="B23" s="149"/>
       <c r="C23" s="26" t="s">
         <v>898</v>
       </c>
@@ -13545,10 +13545,10 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="147">
+      <c r="A24" s="148">
         <v>5</v>
       </c>
-      <c r="B24" s="153" t="s">
+      <c r="B24" s="149" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="28" t="s">
@@ -13562,8 +13562,8 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="147"/>
-      <c r="B25" s="153"/>
+      <c r="A25" s="148"/>
+      <c r="B25" s="149"/>
       <c r="C25" s="26" t="s">
         <v>903</v>
       </c>
@@ -13575,8 +13575,8 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="147"/>
-      <c r="B26" s="153"/>
+      <c r="A26" s="148"/>
+      <c r="B26" s="149"/>
       <c r="C26" s="26" t="s">
         <v>906</v>
       </c>
@@ -13588,8 +13588,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8">
-      <c r="A27" s="147"/>
-      <c r="B27" s="153"/>
+      <c r="A27" s="148"/>
+      <c r="B27" s="149"/>
       <c r="C27" s="28" t="s">
         <v>909</v>
       </c>
@@ -13601,8 +13601,8 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="147"/>
-      <c r="B28" s="153"/>
+      <c r="A28" s="148"/>
+      <c r="B28" s="149"/>
       <c r="C28" s="26" t="s">
         <v>911</v>
       </c>
@@ -13614,10 +13614,10 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="152" t="s">
+      <c r="A29" s="150" t="s">
         <v>914</v>
       </c>
-      <c r="B29" s="153" t="s">
+      <c r="B29" s="149" t="s">
         <v>915</v>
       </c>
       <c r="C29" s="26" t="s">
@@ -13631,8 +13631,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8">
-      <c r="A30" s="152"/>
-      <c r="B30" s="153"/>
+      <c r="A30" s="150"/>
+      <c r="B30" s="149"/>
       <c r="C30" s="26" t="s">
         <v>918</v>
       </c>
@@ -13644,8 +13644,8 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="152"/>
-      <c r="B31" s="153"/>
+      <c r="A31" s="150"/>
+      <c r="B31" s="149"/>
       <c r="C31" s="26" t="s">
         <v>920</v>
       </c>
@@ -13657,10 +13657,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="43.8" thickBot="1">
-      <c r="A32" s="147">
+      <c r="A32" s="148">
         <v>7</v>
       </c>
-      <c r="B32" s="153" t="s">
+      <c r="B32" s="149" t="s">
         <v>86</v>
       </c>
       <c r="C32" s="28" t="s">
@@ -13674,8 +13674,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="58.2" thickBot="1">
-      <c r="A33" s="147"/>
-      <c r="B33" s="153"/>
+      <c r="A33" s="148"/>
+      <c r="B33" s="149"/>
       <c r="C33" s="26" t="s">
         <v>926</v>
       </c>
@@ -13687,8 +13687,8 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="147"/>
-      <c r="B34" s="153"/>
+      <c r="A34" s="148"/>
+      <c r="B34" s="149"/>
       <c r="C34" s="26" t="s">
         <v>929</v>
       </c>
@@ -13700,8 +13700,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.2">
-      <c r="A35" s="147"/>
-      <c r="B35" s="153"/>
+      <c r="A35" s="148"/>
+      <c r="B35" s="149"/>
       <c r="C35" s="28" t="s">
         <v>932</v>
       </c>
@@ -13713,8 +13713,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8">
-      <c r="A36" s="147"/>
-      <c r="B36" s="153"/>
+      <c r="A36" s="148"/>
+      <c r="B36" s="149"/>
       <c r="C36" s="26" t="s">
         <v>935</v>
       </c>
@@ -13726,10 +13726,10 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="152" t="s">
+      <c r="A37" s="150" t="s">
         <v>938</v>
       </c>
-      <c r="B37" s="153" t="s">
+      <c r="B37" s="149" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="32">
@@ -13743,8 +13743,8 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="152"/>
-      <c r="B38" s="153"/>
+      <c r="A38" s="150"/>
+      <c r="B38" s="149"/>
       <c r="C38" s="32">
         <v>576</v>
       </c>
@@ -13756,8 +13756,8 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="152"/>
-      <c r="B39" s="153"/>
+      <c r="A39" s="150"/>
+      <c r="B39" s="149"/>
       <c r="C39" s="32">
         <v>356</v>
       </c>
@@ -13769,8 +13769,8 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="152"/>
-      <c r="B40" s="153"/>
+      <c r="A40" s="150"/>
+      <c r="B40" s="149"/>
       <c r="C40" s="32">
         <v>621</v>
       </c>
@@ -13782,8 +13782,8 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="152"/>
-      <c r="B41" s="153"/>
+      <c r="A41" s="150"/>
+      <c r="B41" s="149"/>
       <c r="C41" s="32">
         <v>179</v>
       </c>
@@ -13795,10 +13795,10 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="152" t="s">
+      <c r="A42" s="150" t="s">
         <v>945</v>
       </c>
-      <c r="B42" s="153" t="s">
+      <c r="B42" s="149" t="s">
         <v>87</v>
       </c>
       <c r="C42" s="27"/>
@@ -13806,8 +13806,8 @@
       <c r="E42" s="32"/>
     </row>
     <row r="43" spans="1:5" s="126" customFormat="1">
-      <c r="A43" s="152"/>
-      <c r="B43" s="153"/>
+      <c r="A43" s="150"/>
+      <c r="B43" s="149"/>
       <c r="C43" s="135" t="s">
         <v>946</v>
       </c>
@@ -13819,8 +13819,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="126" customFormat="1">
-      <c r="A44" s="152"/>
-      <c r="B44" s="153"/>
+      <c r="A44" s="150"/>
+      <c r="B44" s="149"/>
       <c r="C44" s="135" t="s">
         <v>949</v>
       </c>
@@ -13832,10 +13832,10 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="152" t="s">
+      <c r="A45" s="150" t="s">
         <v>952</v>
       </c>
-      <c r="B45" s="153" t="s">
+      <c r="B45" s="149" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="27" t="s">
@@ -13849,8 +13849,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="28.8">
-      <c r="A46" s="152"/>
-      <c r="B46" s="153"/>
+      <c r="A46" s="150"/>
+      <c r="B46" s="149"/>
       <c r="C46" s="26" t="s">
         <v>956</v>
       </c>
@@ -13862,8 +13862,8 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="152"/>
-      <c r="B47" s="153"/>
+      <c r="A47" s="150"/>
+      <c r="B47" s="149"/>
       <c r="C47" s="26" t="s">
         <v>959</v>
       </c>
@@ -13875,8 +13875,8 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="152"/>
-      <c r="B48" s="153"/>
+      <c r="A48" s="150"/>
+      <c r="B48" s="149"/>
       <c r="C48" s="26" t="s">
         <v>962</v>
       </c>
@@ -13888,8 +13888,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="28.8">
-      <c r="A49" s="152"/>
-      <c r="B49" s="153"/>
+      <c r="A49" s="150"/>
+      <c r="B49" s="149"/>
       <c r="C49" s="26" t="s">
         <v>965</v>
       </c>
@@ -13901,8 +13901,8 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="152"/>
-      <c r="B50" s="153"/>
+      <c r="A50" s="150"/>
+      <c r="B50" s="149"/>
       <c r="C50" s="26" t="s">
         <v>968</v>
       </c>
@@ -13914,8 +13914,8 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="152"/>
-      <c r="B51" s="153"/>
+      <c r="A51" s="150"/>
+      <c r="B51" s="149"/>
       <c r="C51" s="26" t="s">
         <v>971</v>
       </c>
@@ -13927,8 +13927,8 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="152"/>
-      <c r="B52" s="153"/>
+      <c r="A52" s="150"/>
+      <c r="B52" s="149"/>
       <c r="C52" s="26" t="s">
         <v>974</v>
       </c>
@@ -13940,8 +13940,8 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="152"/>
-      <c r="B53" s="153"/>
+      <c r="A53" s="150"/>
+      <c r="B53" s="149"/>
       <c r="C53" s="26" t="s">
         <v>977</v>
       </c>
@@ -13953,8 +13953,8 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="152"/>
-      <c r="B54" s="153"/>
+      <c r="A54" s="150"/>
+      <c r="B54" s="149"/>
       <c r="C54" s="26" t="s">
         <v>979</v>
       </c>
@@ -13966,8 +13966,8 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="152"/>
-      <c r="B55" s="153"/>
+      <c r="A55" s="150"/>
+      <c r="B55" s="149"/>
       <c r="C55" s="26" t="s">
         <v>982</v>
       </c>
@@ -13979,10 +13979,10 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="152" t="s">
+      <c r="A56" s="150" t="s">
         <v>984</v>
       </c>
-      <c r="B56" s="153" t="s">
+      <c r="B56" s="149" t="s">
         <v>45</v>
       </c>
       <c r="C56" s="26" t="s">
@@ -13996,8 +13996,8 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="152"/>
-      <c r="B57" s="153"/>
+      <c r="A57" s="150"/>
+      <c r="B57" s="149"/>
       <c r="C57" s="28" t="s">
         <v>988</v>
       </c>
@@ -14009,8 +14009,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.8">
-      <c r="A58" s="152"/>
-      <c r="B58" s="153"/>
+      <c r="A58" s="150"/>
+      <c r="B58" s="149"/>
       <c r="C58" s="13" t="s">
         <v>991</v>
       </c>
@@ -14022,8 +14022,8 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="152"/>
-      <c r="B59" s="153"/>
+      <c r="A59" s="150"/>
+      <c r="B59" s="149"/>
       <c r="C59" s="28" t="s">
         <v>994</v>
       </c>
@@ -14035,8 +14035,8 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="152"/>
-      <c r="B60" s="153"/>
+      <c r="A60" s="150"/>
+      <c r="B60" s="149"/>
       <c r="C60" s="28" t="s">
         <v>997</v>
       </c>
@@ -14048,10 +14048,10 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="152" t="s">
+      <c r="A61" s="150" t="s">
         <v>1000</v>
       </c>
-      <c r="B61" s="153" t="s">
+      <c r="B61" s="149" t="s">
         <v>46</v>
       </c>
       <c r="C61" s="26" t="s">
@@ -14065,8 +14065,8 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="152"/>
-      <c r="B62" s="153"/>
+      <c r="A62" s="150"/>
+      <c r="B62" s="149"/>
       <c r="C62" s="26" t="s">
         <v>1004</v>
       </c>
@@ -14078,8 +14078,8 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="152"/>
-      <c r="B63" s="153"/>
+      <c r="A63" s="150"/>
+      <c r="B63" s="149"/>
       <c r="C63" s="26" t="s">
         <v>1007</v>
       </c>
@@ -14091,10 +14091,10 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="152" t="s">
+      <c r="A64" s="150" t="s">
         <v>1009</v>
       </c>
-      <c r="B64" s="153" t="s">
+      <c r="B64" s="149" t="s">
         <v>61</v>
       </c>
       <c r="C64" s="27" t="s">
@@ -14108,8 +14108,8 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="152"/>
-      <c r="B65" s="153"/>
+      <c r="A65" s="150"/>
+      <c r="B65" s="149"/>
       <c r="C65" s="26" t="s">
         <v>1013</v>
       </c>
@@ -14121,8 +14121,8 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="152"/>
-      <c r="B66" s="153"/>
+      <c r="A66" s="150"/>
+      <c r="B66" s="149"/>
       <c r="C66" s="26" t="s">
         <v>1016</v>
       </c>
@@ -14134,8 +14134,8 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="152"/>
-      <c r="B67" s="153"/>
+      <c r="A67" s="150"/>
+      <c r="B67" s="149"/>
       <c r="C67" s="26" t="s">
         <v>1019</v>
       </c>
@@ -14147,8 +14147,8 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="152"/>
-      <c r="B68" s="153"/>
+      <c r="A68" s="150"/>
+      <c r="B68" s="149"/>
       <c r="C68" s="26" t="s">
         <v>1022</v>
       </c>
@@ -14160,8 +14160,8 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="152"/>
-      <c r="B69" s="153"/>
+      <c r="A69" s="150"/>
+      <c r="B69" s="149"/>
       <c r="C69" s="26" t="s">
         <v>1025</v>
       </c>
@@ -14173,8 +14173,8 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="152"/>
-      <c r="B70" s="153"/>
+      <c r="A70" s="150"/>
+      <c r="B70" s="149"/>
       <c r="C70" s="26" t="s">
         <v>1028</v>
       </c>
@@ -14186,8 +14186,8 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="152"/>
-      <c r="B71" s="153"/>
+      <c r="A71" s="150"/>
+      <c r="B71" s="149"/>
       <c r="C71" s="26" t="s">
         <v>1031</v>
       </c>
@@ -14199,8 +14199,8 @@
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="152"/>
-      <c r="B72" s="153"/>
+      <c r="A72" s="150"/>
+      <c r="B72" s="149"/>
       <c r="C72" s="26" t="s">
         <v>1034</v>
       </c>
@@ -14212,10 +14212,10 @@
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="152" t="s">
+      <c r="A73" s="150" t="s">
         <v>1037</v>
       </c>
-      <c r="B73" s="153" t="s">
+      <c r="B73" s="149" t="s">
         <v>62</v>
       </c>
       <c r="C73" s="26" t="s">
@@ -14229,8 +14229,8 @@
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="152"/>
-      <c r="B74" s="153"/>
+      <c r="A74" s="150"/>
+      <c r="B74" s="149"/>
       <c r="C74" s="26" t="s">
         <v>1041</v>
       </c>
@@ -14242,8 +14242,8 @@
       </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="152"/>
-      <c r="B75" s="153"/>
+      <c r="A75" s="150"/>
+      <c r="B75" s="149"/>
       <c r="C75" s="26" t="s">
         <v>1044</v>
       </c>
@@ -14255,8 +14255,8 @@
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="152"/>
-      <c r="B76" s="153"/>
+      <c r="A76" s="150"/>
+      <c r="B76" s="149"/>
       <c r="C76" s="26" t="s">
         <v>1047</v>
       </c>
@@ -14268,21 +14268,21 @@
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="152" t="s">
+      <c r="A77" s="150" t="s">
         <v>1049</v>
       </c>
-      <c r="B77" s="153" t="s">
+      <c r="B77" s="149" t="s">
         <v>197</v>
       </c>
-      <c r="C77" s="148" t="s">
+      <c r="C77" s="155" t="s">
         <v>1748</v>
       </c>
-      <c r="D77" s="149"/>
-      <c r="E77" s="149"/>
+      <c r="D77" s="156"/>
+      <c r="E77" s="156"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="152"/>
-      <c r="B78" s="153"/>
+      <c r="A78" s="150"/>
+      <c r="B78" s="149"/>
       <c r="C78" s="58" t="s">
         <v>864</v>
       </c>
@@ -14294,8 +14294,8 @@
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="152"/>
-      <c r="B79" s="153"/>
+      <c r="A79" s="150"/>
+      <c r="B79" s="149"/>
       <c r="C79" s="58" t="s">
         <v>1722</v>
       </c>
@@ -14307,8 +14307,8 @@
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="152"/>
-      <c r="B80" s="153"/>
+      <c r="A80" s="150"/>
+      <c r="B80" s="149"/>
       <c r="C80" s="58" t="s">
         <v>1057</v>
       </c>
@@ -14320,8 +14320,8 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="152"/>
-      <c r="B81" s="153"/>
+      <c r="A81" s="150"/>
+      <c r="B81" s="149"/>
       <c r="C81" s="58" t="s">
         <v>861</v>
       </c>
@@ -14333,8 +14333,8 @@
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="152"/>
-      <c r="B82" s="153"/>
+      <c r="A82" s="150"/>
+      <c r="B82" s="149"/>
       <c r="C82" s="58" t="s">
         <v>854</v>
       </c>
@@ -14346,8 +14346,8 @@
       </c>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="152"/>
-      <c r="B83" s="153"/>
+      <c r="A83" s="150"/>
+      <c r="B83" s="149"/>
       <c r="C83" s="58" t="s">
         <v>1731</v>
       </c>
@@ -14359,8 +14359,8 @@
       </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="152"/>
-      <c r="B84" s="153"/>
+      <c r="A84" s="150"/>
+      <c r="B84" s="149"/>
       <c r="C84" s="58" t="s">
         <v>859</v>
       </c>
@@ -14372,8 +14372,8 @@
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="152"/>
-      <c r="B85" s="153"/>
+      <c r="A85" s="150"/>
+      <c r="B85" s="149"/>
       <c r="C85" s="58" t="s">
         <v>1736</v>
       </c>
@@ -14385,8 +14385,8 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="152"/>
-      <c r="B86" s="153"/>
+      <c r="A86" s="150"/>
+      <c r="B86" s="149"/>
       <c r="C86" s="58" t="s">
         <v>1739</v>
       </c>
@@ -14398,8 +14398,8 @@
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="152"/>
-      <c r="B87" s="153"/>
+      <c r="A87" s="150"/>
+      <c r="B87" s="149"/>
       <c r="C87" s="58" t="s">
         <v>1742</v>
       </c>
@@ -14411,8 +14411,8 @@
       </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="152"/>
-      <c r="B88" s="153"/>
+      <c r="A88" s="150"/>
+      <c r="B88" s="149"/>
       <c r="C88" s="58" t="s">
         <v>1745</v>
       </c>
@@ -14424,17 +14424,17 @@
       </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="152"/>
-      <c r="B89" s="153"/>
-      <c r="C89" s="148" t="s">
+      <c r="A89" s="150"/>
+      <c r="B89" s="149"/>
+      <c r="C89" s="155" t="s">
         <v>1749</v>
       </c>
-      <c r="D89" s="149"/>
-      <c r="E89" s="149"/>
+      <c r="D89" s="156"/>
+      <c r="E89" s="156"/>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="152"/>
-      <c r="B90" s="153"/>
+      <c r="A90" s="150"/>
+      <c r="B90" s="149"/>
       <c r="C90" s="26" t="s">
         <v>698</v>
       </c>
@@ -14446,8 +14446,8 @@
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="152"/>
-      <c r="B91" s="153"/>
+      <c r="A91" s="150"/>
+      <c r="B91" s="149"/>
       <c r="C91" s="26" t="s">
         <v>859</v>
       </c>
@@ -14459,8 +14459,8 @@
       </c>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="152"/>
-      <c r="B92" s="153"/>
+      <c r="A92" s="150"/>
+      <c r="B92" s="149"/>
       <c r="C92" s="26" t="s">
         <v>847</v>
       </c>
@@ -14472,8 +14472,8 @@
       </c>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="152"/>
-      <c r="B93" s="153"/>
+      <c r="A93" s="150"/>
+      <c r="B93" s="149"/>
       <c r="C93" s="26" t="s">
         <v>861</v>
       </c>
@@ -14485,8 +14485,8 @@
       </c>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="152"/>
-      <c r="B94" s="153"/>
+      <c r="A94" s="150"/>
+      <c r="B94" s="149"/>
       <c r="C94" s="26" t="s">
         <v>852</v>
       </c>
@@ -14498,8 +14498,8 @@
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="152"/>
-      <c r="B95" s="153"/>
+      <c r="A95" s="150"/>
+      <c r="B95" s="149"/>
       <c r="C95" s="26" t="s">
         <v>951</v>
       </c>
@@ -14511,8 +14511,8 @@
       </c>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="152"/>
-      <c r="B96" s="153"/>
+      <c r="A96" s="150"/>
+      <c r="B96" s="149"/>
       <c r="C96" s="26" t="s">
         <v>1057</v>
       </c>
@@ -14524,8 +14524,8 @@
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="152"/>
-      <c r="B97" s="153"/>
+      <c r="A97" s="150"/>
+      <c r="B97" s="149"/>
       <c r="C97" s="26" t="s">
         <v>1059</v>
       </c>
@@ -14537,10 +14537,10 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="152" t="s">
+      <c r="A98" s="150" t="s">
         <v>1060</v>
       </c>
-      <c r="B98" s="153" t="s">
+      <c r="B98" s="149" t="s">
         <v>49</v>
       </c>
       <c r="C98" s="26" t="s">
@@ -14554,8 +14554,8 @@
       </c>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="152"/>
-      <c r="B99" s="153"/>
+      <c r="A99" s="150"/>
+      <c r="B99" s="149"/>
       <c r="C99" s="26" t="s">
         <v>1064</v>
       </c>
@@ -14567,8 +14567,8 @@
       </c>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="152"/>
-      <c r="B100" s="153"/>
+      <c r="A100" s="150"/>
+      <c r="B100" s="149"/>
       <c r="C100" s="26" t="s">
         <v>1067</v>
       </c>
@@ -14580,10 +14580,10 @@
       </c>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="152" t="s">
+      <c r="A101" s="150" t="s">
         <v>1071</v>
       </c>
-      <c r="B101" s="153" t="s">
+      <c r="B101" s="149" t="s">
         <v>59</v>
       </c>
       <c r="C101" s="26" t="s">
@@ -14597,8 +14597,8 @@
       </c>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="152"/>
-      <c r="B102" s="153"/>
+      <c r="A102" s="150"/>
+      <c r="B102" s="149"/>
       <c r="C102" s="26" t="s">
         <v>1075</v>
       </c>
@@ -14610,8 +14610,8 @@
       </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="152"/>
-      <c r="B103" s="153"/>
+      <c r="A103" s="150"/>
+      <c r="B103" s="149"/>
       <c r="C103" s="26" t="s">
         <v>1078</v>
       </c>
@@ -14623,8 +14623,8 @@
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="152"/>
-      <c r="B104" s="153"/>
+      <c r="A104" s="150"/>
+      <c r="B104" s="149"/>
       <c r="C104" s="26" t="s">
         <v>1081</v>
       </c>
@@ -14636,10 +14636,10 @@
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="152" t="s">
+      <c r="A105" s="150" t="s">
         <v>1084</v>
       </c>
-      <c r="B105" s="153" t="s">
+      <c r="B105" s="149" t="s">
         <v>68</v>
       </c>
       <c r="C105" s="27" t="s">
@@ -14653,8 +14653,8 @@
       </c>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="152"/>
-      <c r="B106" s="153"/>
+      <c r="A106" s="150"/>
+      <c r="B106" s="149"/>
       <c r="C106" s="26" t="s">
         <v>1088</v>
       </c>
@@ -14666,10 +14666,10 @@
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="152" t="s">
+      <c r="A107" s="150" t="s">
         <v>1091</v>
       </c>
-      <c r="B107" s="153" t="s">
+      <c r="B107" s="149" t="s">
         <v>73</v>
       </c>
       <c r="C107" s="26" t="s">
@@ -14683,8 +14683,8 @@
       </c>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="152"/>
-      <c r="B108" s="153"/>
+      <c r="A108" s="150"/>
+      <c r="B108" s="149"/>
       <c r="C108" s="26" t="s">
         <v>1095</v>
       </c>
@@ -14696,10 +14696,10 @@
       </c>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="152" t="s">
+      <c r="A109" s="150" t="s">
         <v>1097</v>
       </c>
-      <c r="B109" s="153" t="s">
+      <c r="B109" s="149" t="s">
         <v>70</v>
       </c>
       <c r="C109" s="26" t="s">
@@ -14713,8 +14713,8 @@
       </c>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="152"/>
-      <c r="B110" s="153"/>
+      <c r="A110" s="150"/>
+      <c r="B110" s="149"/>
       <c r="C110" s="26" t="s">
         <v>1101</v>
       </c>
@@ -14726,8 +14726,8 @@
       </c>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="152"/>
-      <c r="B111" s="153"/>
+      <c r="A111" s="150"/>
+      <c r="B111" s="149"/>
       <c r="C111" s="26" t="s">
         <v>1103</v>
       </c>
@@ -14739,8 +14739,8 @@
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="152"/>
-      <c r="B112" s="153"/>
+      <c r="A112" s="150"/>
+      <c r="B112" s="149"/>
       <c r="C112" s="26" t="s">
         <v>1106</v>
       </c>
@@ -14752,10 +14752,10 @@
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="152" t="s">
+      <c r="A113" s="150" t="s">
         <v>1595</v>
       </c>
-      <c r="B113" s="153" t="s">
+      <c r="B113" s="149" t="s">
         <v>32</v>
       </c>
       <c r="C113" s="26" t="s">
@@ -14767,8 +14767,8 @@
       <c r="E113" s="26"/>
     </row>
     <row r="114" spans="1:6">
-      <c r="A114" s="152"/>
-      <c r="B114" s="153"/>
+      <c r="A114" s="150"/>
+      <c r="B114" s="149"/>
       <c r="C114" s="26" t="s">
         <v>1681</v>
       </c>
@@ -14778,8 +14778,8 @@
       <c r="E114" s="26"/>
     </row>
     <row r="115" spans="1:6">
-      <c r="A115" s="152"/>
-      <c r="B115" s="153"/>
+      <c r="A115" s="150"/>
+      <c r="B115" s="149"/>
       <c r="C115" s="124" t="s">
         <v>2140</v>
       </c>
@@ -14789,8 +14789,8 @@
       <c r="E115" s="26"/>
     </row>
     <row r="116" spans="1:6">
-      <c r="A116" s="152"/>
-      <c r="B116" s="153"/>
+      <c r="A116" s="150"/>
+      <c r="B116" s="149"/>
       <c r="C116" s="26" t="s">
         <v>1682</v>
       </c>
@@ -14800,8 +14800,8 @@
       <c r="E116" s="26"/>
     </row>
     <row r="117" spans="1:6">
-      <c r="A117" s="152"/>
-      <c r="B117" s="153"/>
+      <c r="A117" s="150"/>
+      <c r="B117" s="149"/>
       <c r="C117" s="26" t="s">
         <v>1683</v>
       </c>
@@ -14811,10 +14811,10 @@
       <c r="E117" s="26"/>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="152" t="s">
+      <c r="A118" s="150" t="s">
         <v>1597</v>
       </c>
-      <c r="B118" s="153" t="s">
+      <c r="B118" s="149" t="s">
         <v>34</v>
       </c>
       <c r="C118" s="26" t="s">
@@ -14826,8 +14826,8 @@
       <c r="E118" s="26"/>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="152"/>
-      <c r="B119" s="153"/>
+      <c r="A119" s="150"/>
+      <c r="B119" s="149"/>
       <c r="C119" s="26" t="s">
         <v>1689</v>
       </c>
@@ -14837,8 +14837,8 @@
       <c r="E119" s="26"/>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="152"/>
-      <c r="B120" s="153"/>
+      <c r="A120" s="150"/>
+      <c r="B120" s="149"/>
       <c r="C120" s="26" t="s">
         <v>1690</v>
       </c>
@@ -14848,10 +14848,10 @@
       <c r="E120" s="26"/>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="152" t="s">
+      <c r="A121" s="150" t="s">
         <v>1599</v>
       </c>
-      <c r="B121" s="153" t="s">
+      <c r="B121" s="149" t="s">
         <v>22</v>
       </c>
       <c r="C121" s="26" t="s">
@@ -14868,8 +14868,8 @@
       </c>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="152"/>
-      <c r="B122" s="153"/>
+      <c r="A122" s="150"/>
+      <c r="B122" s="149"/>
       <c r="C122" s="26" t="s">
         <v>1694</v>
       </c>
@@ -14884,8 +14884,8 @@
       </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="152"/>
-      <c r="B123" s="153"/>
+      <c r="A123" s="150"/>
+      <c r="B123" s="149"/>
       <c r="C123" s="26" t="s">
         <v>1695</v>
       </c>
@@ -14900,8 +14900,8 @@
       </c>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="152"/>
-      <c r="B124" s="153"/>
+      <c r="A124" s="150"/>
+      <c r="B124" s="149"/>
       <c r="C124" s="26" t="s">
         <v>1696</v>
       </c>
@@ -14916,8 +14916,8 @@
       </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="152"/>
-      <c r="B125" s="153"/>
+      <c r="A125" s="150"/>
+      <c r="B125" s="149"/>
       <c r="C125" s="26" t="s">
         <v>1697</v>
       </c>
@@ -14932,8 +14932,8 @@
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="152"/>
-      <c r="B126" s="153"/>
+      <c r="A126" s="150"/>
+      <c r="B126" s="149"/>
       <c r="C126" s="26" t="s">
         <v>1698</v>
       </c>
@@ -14948,8 +14948,8 @@
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="152"/>
-      <c r="B127" s="153"/>
+      <c r="A127" s="150"/>
+      <c r="B127" s="149"/>
       <c r="C127" s="13" t="s">
         <v>1699</v>
       </c>
@@ -14964,8 +14964,8 @@
       </c>
     </row>
     <row r="128" spans="1:6">
-      <c r="A128" s="152"/>
-      <c r="B128" s="153"/>
+      <c r="A128" s="150"/>
+      <c r="B128" s="149"/>
       <c r="C128" s="28" t="s">
         <v>1700</v>
       </c>
@@ -14980,8 +14980,8 @@
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" s="152"/>
-      <c r="B129" s="153"/>
+      <c r="A129" s="150"/>
+      <c r="B129" s="149"/>
       <c r="C129" s="28" t="s">
         <v>1701</v>
       </c>
@@ -14996,10 +14996,10 @@
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="A130" s="154">
+      <c r="A130" s="157">
         <v>25</v>
       </c>
-      <c r="B130" s="154" t="s">
+      <c r="B130" s="157" t="s">
         <v>1752</v>
       </c>
       <c r="C130" s="10" t="s">
@@ -15059,7 +15059,7 @@
       <c r="A138" s="146">
         <v>26</v>
       </c>
-      <c r="B138" s="147" t="s">
+      <c r="B138" s="148" t="s">
         <v>1761</v>
       </c>
       <c r="C138" s="13" t="s">
@@ -15071,7 +15071,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="146"/>
-      <c r="B139" s="147"/>
+      <c r="B139" s="148"/>
       <c r="C139" s="13" t="s">
         <v>1764</v>
       </c>
@@ -15081,7 +15081,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="146"/>
-      <c r="B140" s="147"/>
+      <c r="B140" s="148"/>
       <c r="C140" s="13" t="s">
         <v>1047</v>
       </c>
@@ -15093,7 +15093,7 @@
       <c r="A141" s="146">
         <v>27</v>
       </c>
-      <c r="B141" s="147" t="s">
+      <c r="B141" s="148" t="s">
         <v>1791</v>
       </c>
       <c r="C141" s="13" t="s">
@@ -15108,7 +15108,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="146"/>
-      <c r="B142" s="147"/>
+      <c r="B142" s="148"/>
       <c r="C142" s="13" t="s">
         <v>1769</v>
       </c>
@@ -15121,7 +15121,7 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="146"/>
-      <c r="B143" s="147"/>
+      <c r="B143" s="148"/>
       <c r="C143" s="13" t="s">
         <v>1772</v>
       </c>
@@ -15134,7 +15134,7 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="146"/>
-      <c r="B144" s="147"/>
+      <c r="B144" s="148"/>
       <c r="C144" s="13" t="s">
         <v>1775</v>
       </c>
@@ -15147,7 +15147,7 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="146"/>
-      <c r="B145" s="147"/>
+      <c r="B145" s="148"/>
       <c r="C145" s="13" t="s">
         <v>1778</v>
       </c>
@@ -15160,7 +15160,7 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="146"/>
-      <c r="B146" s="147"/>
+      <c r="B146" s="148"/>
       <c r="C146" s="13" t="s">
         <v>1781</v>
       </c>
@@ -15173,7 +15173,7 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="146"/>
-      <c r="B147" s="147"/>
+      <c r="B147" s="148"/>
       <c r="C147" s="13" t="s">
         <v>1784</v>
       </c>
@@ -15186,7 +15186,7 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="146"/>
-      <c r="B148" s="147"/>
+      <c r="B148" s="148"/>
       <c r="C148" s="13" t="s">
         <v>1787</v>
       </c>
@@ -15199,7 +15199,7 @@
     </row>
     <row r="149" spans="1:5" ht="28.8">
       <c r="A149" s="146"/>
-      <c r="B149" s="147"/>
+      <c r="B149" s="148"/>
       <c r="C149" s="13" t="s">
         <v>845</v>
       </c>
@@ -15214,41 +15214,41 @@
       <c r="A150" s="146">
         <v>28</v>
       </c>
-      <c r="B150" s="151" t="s">
+      <c r="B150" s="159" t="s">
         <v>196</v>
       </c>
-      <c r="C150" s="148" t="s">
+      <c r="C150" s="155" t="s">
         <v>1749</v>
       </c>
-      <c r="D150" s="149"/>
-      <c r="E150" s="149"/>
+      <c r="D150" s="156"/>
+      <c r="E150" s="156"/>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="146"/>
-      <c r="B151" s="151"/>
-      <c r="C151" s="150" t="s">
+      <c r="B151" s="159"/>
+      <c r="C151" s="158" t="s">
         <v>1799</v>
       </c>
-      <c r="D151" s="150"/>
-      <c r="E151" s="150"/>
+      <c r="D151" s="158"/>
+      <c r="E151" s="158"/>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="146"/>
-      <c r="B152" s="151"/>
-      <c r="C152" s="148" t="s">
+      <c r="B152" s="159"/>
+      <c r="C152" s="155" t="s">
         <v>1748</v>
       </c>
-      <c r="D152" s="149"/>
-      <c r="E152" s="149"/>
+      <c r="D152" s="156"/>
+      <c r="E152" s="156"/>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="146"/>
-      <c r="B153" s="151"/>
-      <c r="C153" s="150" t="s">
+      <c r="B153" s="159"/>
+      <c r="C153" s="158" t="s">
         <v>1800</v>
       </c>
-      <c r="D153" s="150"/>
-      <c r="E153" s="150"/>
+      <c r="D153" s="158"/>
+      <c r="E153" s="158"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="56">
@@ -15268,7 +15268,7 @@
       <c r="A155" s="56">
         <v>30</v>
       </c>
-      <c r="B155" s="147" t="s">
+      <c r="B155" s="148" t="s">
         <v>42</v>
       </c>
       <c r="C155" s="80" t="s">
@@ -15282,7 +15282,7 @@
       </c>
     </row>
     <row r="156" spans="1:5">
-      <c r="B156" s="147"/>
+      <c r="B156" s="148"/>
       <c r="C156" s="80" t="s">
         <v>1839</v>
       </c>
@@ -15294,7 +15294,7 @@
       </c>
     </row>
     <row r="157" spans="1:5" ht="28.8">
-      <c r="B157" s="147"/>
+      <c r="B157" s="148"/>
       <c r="C157" s="80" t="s">
         <v>1841</v>
       </c>
@@ -15306,7 +15306,7 @@
       </c>
     </row>
     <row r="158" spans="1:5" ht="43.2">
-      <c r="B158" s="147"/>
+      <c r="B158" s="148"/>
       <c r="C158" s="80" t="s">
         <v>1844</v>
       </c>
@@ -15318,7 +15318,7 @@
       </c>
     </row>
     <row r="159" spans="1:5" ht="28.8">
-      <c r="B159" s="147"/>
+      <c r="B159" s="148"/>
       <c r="C159" s="80" t="s">
         <v>1847</v>
       </c>
@@ -15330,7 +15330,7 @@
       </c>
     </row>
     <row r="160" spans="1:5" ht="43.2">
-      <c r="B160" s="147"/>
+      <c r="B160" s="148"/>
       <c r="C160" s="80" t="s">
         <v>1850</v>
       </c>
@@ -15342,7 +15342,7 @@
       </c>
     </row>
     <row r="161" spans="1:5" ht="28.8">
-      <c r="B161" s="147"/>
+      <c r="B161" s="148"/>
       <c r="C161" s="80" t="s">
         <v>1853</v>
       </c>
@@ -15354,7 +15354,7 @@
       </c>
     </row>
     <row r="162" spans="1:5" ht="28.8">
-      <c r="B162" s="147"/>
+      <c r="B162" s="148"/>
       <c r="C162" s="80" t="s">
         <v>1856</v>
       </c>
@@ -15366,7 +15366,7 @@
       </c>
     </row>
     <row r="163" spans="1:5" ht="28.8">
-      <c r="B163" s="147"/>
+      <c r="B163" s="148"/>
       <c r="C163" s="80" t="s">
         <v>1859</v>
       </c>
@@ -15378,7 +15378,7 @@
       </c>
     </row>
     <row r="164" spans="1:5" ht="28.8">
-      <c r="B164" s="147"/>
+      <c r="B164" s="148"/>
       <c r="C164" s="80" t="s">
         <v>1862</v>
       </c>
@@ -15390,7 +15390,7 @@
       </c>
     </row>
     <row r="165" spans="1:5" ht="28.8">
-      <c r="B165" s="147"/>
+      <c r="B165" s="148"/>
       <c r="C165" s="80" t="s">
         <v>1865</v>
       </c>
@@ -15402,7 +15402,7 @@
       </c>
     </row>
     <row r="166" spans="1:5" ht="28.8">
-      <c r="B166" s="147"/>
+      <c r="B166" s="148"/>
       <c r="C166" s="80" t="s">
         <v>1868</v>
       </c>
@@ -15414,7 +15414,7 @@
       </c>
     </row>
     <row r="167" spans="1:5">
-      <c r="B167" s="147"/>
+      <c r="B167" s="148"/>
       <c r="C167" s="80" t="s">
         <v>1871</v>
       </c>
@@ -15426,7 +15426,7 @@
       </c>
     </row>
     <row r="168" spans="1:5">
-      <c r="B168" s="147"/>
+      <c r="B168" s="148"/>
       <c r="C168" s="80" t="s">
         <v>1874</v>
       </c>
@@ -15441,7 +15441,7 @@
       <c r="A169" s="56">
         <v>31</v>
       </c>
-      <c r="B169" s="147" t="s">
+      <c r="B169" s="148" t="s">
         <v>1935</v>
       </c>
       <c r="C169" s="87" t="s">
@@ -15450,7 +15450,7 @@
       <c r="D169" s="88"/>
     </row>
     <row r="170" spans="1:5">
-      <c r="B170" s="147"/>
+      <c r="B170" s="148"/>
       <c r="C170" s="87" t="s">
         <v>1938</v>
       </c>
@@ -15459,7 +15459,7 @@
       <c r="A171" s="146">
         <v>32</v>
       </c>
-      <c r="B171" s="147" t="s">
+      <c r="B171" s="148" t="s">
         <v>2136</v>
       </c>
       <c r="C171" s="87" t="s">
@@ -15468,14 +15468,14 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="146"/>
-      <c r="B172" s="147"/>
+      <c r="B172" s="148"/>
       <c r="C172" s="87" t="s">
         <v>2138</v>
       </c>
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="146"/>
-      <c r="B173" s="147"/>
+      <c r="B173" s="148"/>
       <c r="C173" s="87" t="s">
         <v>2139</v>
       </c>
@@ -15484,7 +15484,7 @@
       <c r="A174" s="138">
         <v>34</v>
       </c>
-      <c r="B174" s="159" t="s">
+      <c r="B174" s="147" t="s">
         <v>2194</v>
       </c>
       <c r="C174" s="139" t="s">
@@ -15499,7 +15499,7 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="138"/>
-      <c r="B175" s="159"/>
+      <c r="B175" s="147"/>
       <c r="C175" s="139" t="s">
         <v>2180</v>
       </c>
@@ -15512,7 +15512,7 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="138"/>
-      <c r="B176" s="159"/>
+      <c r="B176" s="147"/>
       <c r="C176" s="139" t="s">
         <v>2181</v>
       </c>
@@ -15525,7 +15525,7 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" s="138"/>
-      <c r="B177" s="159"/>
+      <c r="B177" s="147"/>
       <c r="C177" s="139" t="s">
         <v>2200</v>
       </c>
@@ -15538,7 +15538,7 @@
     </row>
     <row r="178" spans="1:6" ht="28.8">
       <c r="A178" s="138"/>
-      <c r="B178" s="159"/>
+      <c r="B178" s="147"/>
       <c r="C178" s="139" t="s">
         <v>2203</v>
       </c>
@@ -15551,7 +15551,7 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" s="138"/>
-      <c r="B179" s="159"/>
+      <c r="B179" s="147"/>
       <c r="C179" s="139" t="s">
         <v>2182</v>
       </c>
@@ -15564,7 +15564,7 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" s="138"/>
-      <c r="B180" s="159"/>
+      <c r="B180" s="147"/>
       <c r="C180" s="139" t="s">
         <v>2205</v>
       </c>
@@ -15576,7 +15576,7 @@
       </c>
     </row>
     <row r="181" spans="1:6">
-      <c r="B181" s="159"/>
+      <c r="B181" s="147"/>
       <c r="C181" s="139" t="s">
         <v>2206</v>
       </c>
@@ -15592,8 +15592,8 @@
       <c r="A182" s="56">
         <v>35</v>
       </c>
-      <c r="B182" s="159" t="s">
-        <v>2223</v>
+      <c r="B182" s="147" t="s">
+        <v>2222</v>
       </c>
       <c r="C182" s="139" t="s">
         <v>2208</v>
@@ -15606,7 +15606,7 @@
       </c>
     </row>
     <row r="183" spans="1:6">
-      <c r="B183" s="159"/>
+      <c r="B183" s="147"/>
       <c r="C183" s="139" t="s">
         <v>2210</v>
       </c>
@@ -15618,7 +15618,7 @@
       </c>
     </row>
     <row r="184" spans="1:6">
-      <c r="B184" s="159"/>
+      <c r="B184" s="147"/>
       <c r="C184" s="139" t="s">
         <v>2206</v>
       </c>
@@ -15630,7 +15630,7 @@
       </c>
     </row>
     <row r="185" spans="1:6">
-      <c r="B185" s="159"/>
+      <c r="B185" s="147"/>
       <c r="C185" s="139" t="s">
         <v>1874</v>
       </c>
@@ -15646,6 +15646,56 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="B171:B173"/>
+    <mergeCell ref="A171:A173"/>
+    <mergeCell ref="B169:B170"/>
+    <mergeCell ref="A150:A153"/>
+    <mergeCell ref="B155:B168"/>
+    <mergeCell ref="C150:E150"/>
+    <mergeCell ref="C151:E151"/>
+    <mergeCell ref="C152:E152"/>
+    <mergeCell ref="C153:E153"/>
+    <mergeCell ref="B150:B153"/>
+    <mergeCell ref="B138:B140"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="A113:A117"/>
+    <mergeCell ref="B113:B117"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="B118:B120"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="A101:A104"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="B130:B137"/>
+    <mergeCell ref="A130:A137"/>
+    <mergeCell ref="A121:A129"/>
+    <mergeCell ref="B121:B129"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="A109:A112"/>
+    <mergeCell ref="B109:B112"/>
+    <mergeCell ref="A64:A72"/>
+    <mergeCell ref="B64:B72"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="A77:A97"/>
+    <mergeCell ref="B77:B97"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
     <mergeCell ref="B174:B181"/>
     <mergeCell ref="B182:B185"/>
     <mergeCell ref="A32:A36"/>
@@ -15662,56 +15712,6 @@
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="A61:A63"/>
     <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="A64:A72"/>
-    <mergeCell ref="B64:B72"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="A77:A97"/>
-    <mergeCell ref="B77:B97"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="A109:A112"/>
-    <mergeCell ref="B109:B112"/>
-    <mergeCell ref="B138:B140"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="A113:A117"/>
-    <mergeCell ref="B113:B117"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="B118:B120"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="A101:A104"/>
-    <mergeCell ref="B101:B104"/>
-    <mergeCell ref="B130:B137"/>
-    <mergeCell ref="A130:A137"/>
-    <mergeCell ref="A121:A129"/>
-    <mergeCell ref="B121:B129"/>
-    <mergeCell ref="C150:E150"/>
-    <mergeCell ref="C151:E151"/>
-    <mergeCell ref="C152:E152"/>
-    <mergeCell ref="C153:E153"/>
-    <mergeCell ref="B150:B153"/>
-    <mergeCell ref="B171:B173"/>
-    <mergeCell ref="A171:A173"/>
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="A150:A153"/>
-    <mergeCell ref="B155:B168"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15785,7 +15785,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8">
-      <c r="A3" s="151"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="63" t="s">
         <v>129</v>
       </c>
@@ -15806,7 +15806,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="151"/>
+      <c r="A4" s="159"/>
       <c r="B4" s="63" t="s">
         <v>132</v>
       </c>
@@ -15827,7 +15827,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="130" customFormat="1" ht="28.8">
-      <c r="A5" s="151"/>
+      <c r="A5" s="159"/>
       <c r="B5" s="127" t="s">
         <v>135</v>
       </c>
@@ -15848,7 +15848,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="151"/>
+      <c r="A6" s="159"/>
       <c r="B6" s="63" t="s">
         <v>137</v>
       </c>
@@ -15869,7 +15869,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8">
-      <c r="A7" s="151"/>
+      <c r="A7" s="159"/>
       <c r="B7" s="63" t="s">
         <v>140</v>
       </c>
@@ -15890,7 +15890,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2">
-      <c r="A8" s="151"/>
+      <c r="A8" s="159"/>
       <c r="B8" s="66" t="s">
         <v>142</v>
       </c>
@@ -15911,7 +15911,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8">
-      <c r="A9" s="151"/>
+      <c r="A9" s="159"/>
       <c r="B9" s="66" t="s">
         <v>144</v>
       </c>
@@ -15932,7 +15932,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A10" s="151"/>
+      <c r="A10" s="159"/>
       <c r="B10" s="74" t="s">
         <v>145</v>
       </c>
@@ -15953,7 +15953,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A11" s="151"/>
+      <c r="A11" s="159"/>
       <c r="B11" s="74" t="s">
         <v>146</v>
       </c>
@@ -15974,7 +15974,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A12" s="151"/>
+      <c r="A12" s="159"/>
       <c r="B12" s="74" t="s">
         <v>148</v>
       </c>
@@ -15995,7 +15995,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A13" s="151"/>
+      <c r="A13" s="159"/>
       <c r="B13" s="74" t="s">
         <v>150</v>
       </c>
@@ -16016,7 +16016,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.2">
-      <c r="A14" s="151"/>
+      <c r="A14" s="159"/>
       <c r="B14" s="66" t="s">
         <v>151</v>
       </c>
@@ -16037,7 +16037,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.2">
-      <c r="A15" s="151"/>
+      <c r="A15" s="159"/>
       <c r="B15" s="66" t="s">
         <v>154</v>
       </c>
@@ -16058,7 +16058,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="43.2">
-      <c r="A16" s="151"/>
+      <c r="A16" s="159"/>
       <c r="B16" s="66" t="s">
         <v>156</v>
       </c>
@@ -16079,7 +16079,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="100.8">
-      <c r="A17" s="151"/>
+      <c r="A17" s="159"/>
       <c r="B17" s="66" t="s">
         <v>158</v>
       </c>
@@ -21425,18 +21425,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21459,14 +21459,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F835A65A-8852-436B-8C93-990B831CCA81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34169AE6-2D3A-46F3-9DCC-17D5C75F3D70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="fa0a58a8-6aee-41ea-a8cf-318e5bdc9d94"/>
@@ -21481,4 +21473,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F835A65A-8852-436B-8C93-990B831CCA81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>